<commit_message>
fix bug with intervention type
</commit_message>
<xml_diff>
--- a/Data Extraction Sheet.xlsx
+++ b/Data Extraction Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/rw3031_cumc_columbia_edu/Documents/Documents/EveryBreathMatters/systematic review/lungcancer_tech_slr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7373493-5A43-43BB-BCA3-0DE686A9F3B9}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E48A93FB-69D0-4F8F-AC14-242F189C0B09}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1801,9 +1801,6 @@
     <t>wearable device</t>
   </si>
   <si>
-    <t xml:space="preserve">Intervention Type </t>
-  </si>
-  <si>
     <t>both</t>
   </si>
   <si>
@@ -2072,6 +2069,9 @@
   </si>
   <si>
     <t>promotion of healthy behavior</t>
+  </si>
+  <si>
+    <t>Intervention_type</t>
   </si>
 </sst>
 </file>
@@ -3030,8 +3030,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3305175" y="184150"/>
-              <a:ext cx="4581526" cy="3041650"/>
+              <a:off x="3302000" y="180975"/>
+              <a:ext cx="4584701" cy="2990850"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3197,7 +3197,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E50D8823-D66D-486C-A66C-0129AAC9EB4E}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E50D8823-D66D-486C-A66C-0129AAC9EB4E}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C1:D14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" numFmtId="49" showAll="0">
@@ -3283,8 +3283,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{828B0BCE-3BFA-4916-81DC-E50F5CA6D7E6}" name="Table2" displayName="Table2" ref="A1:W296" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:W296" xr:uid="{828B0BCE-3BFA-4916-81DC-E50F5CA6D7E6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W200">
-    <sortCondition ref="C1:C296"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W296">
+    <sortCondition ref="A1:A296"/>
   </sortState>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{3FCD09ED-4669-4B6A-AA10-CA8EEB1F9114}" name="ID"/>
@@ -3323,7 +3323,7 @@
     <tableColumn id="2" xr3:uid="{D63BE219-238D-499A-A804-1C9D67AC2E34}" name="Challenges of technology use"/>
     <tableColumn id="3" xr3:uid="{8D569B08-204B-49B5-9725-B30BDDB921A6}" name="Findings"/>
     <tableColumn id="4" xr3:uid="{95CB8623-0E1E-463A-832C-23B54764F2AC}" name="Study limitations"/>
-    <tableColumn id="5" xr3:uid="{53D772CB-9168-4CE8-B089-683C24EB7C05}" name="Intervention Type "/>
+    <tableColumn id="5" xr3:uid="{53D772CB-9168-4CE8-B089-683C24EB7C05}" name="Intervention_type"/>
     <tableColumn id="6" xr3:uid="{0EAFCAAA-2D49-48B0-8A7A-2A41463DA5AF}" name="Length (in months)"/>
     <tableColumn id="7" xr3:uid="{29717171-C5A6-45AA-857D-97ACBB2CA000}" name="Treatment 2"/>
     <tableColumn id="8" xr3:uid="{7A49C9F5-5988-4F1A-AD3C-EE8AEC3F28B7}" name="Pre_post"/>
@@ -3613,10 +3613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF200"/>
+  <dimension ref="A1:AF296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="198" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3647,7 +3647,7 @@
     <col min="25" max="25" width="38.36328125" customWidth="1"/>
     <col min="26" max="26" width="34.54296875" customWidth="1"/>
     <col min="27" max="27" width="49.26953125" customWidth="1"/>
-    <col min="28" max="28" width="21.81640625" customWidth="1"/>
+    <col min="28" max="28" width="59.1796875" customWidth="1"/>
     <col min="30" max="30" width="14.453125" customWidth="1"/>
     <col min="31" max="31" width="14.7265625" customWidth="1"/>
   </cols>
@@ -3699,7 +3699,7 @@
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>14</v>
@@ -3720,7 +3720,7 @@
         <v>19</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>21</v>
@@ -3734,91 +3734,91 @@
       <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>519</v>
+      <c r="AB1" s="21" t="s">
+        <v>609</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AE1" s="21" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AF1" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="C2">
-        <v>2007</v>
+        <v>2023</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>528</v>
       </c>
       <c r="H2" t="s">
-        <v>460</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>533</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>532</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>191</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>194</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>187</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
+        <v>546</v>
+      </c>
+      <c r="P2" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" t="s">
-        <v>192</v>
-      </c>
-      <c r="S2" t="s">
-        <v>188</v>
-      </c>
-      <c r="T2" t="s">
-        <v>193</v>
-      </c>
-      <c r="U2" t="s">
-        <v>560</v>
-      </c>
-      <c r="V2" t="s">
-        <v>189</v>
-      </c>
       <c r="W2" s="20" t="s">
-        <v>561</v>
+        <v>574</v>
       </c>
       <c r="X2" t="s">
         <v>41</v>
@@ -3832,91 +3832,91 @@
       <c r="AA2" t="s">
         <v>44</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC2">
         <v>3</v>
       </c>
       <c r="AD2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AE2" s="20" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AF2" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>2007</v>
+        <v>2024</v>
       </c>
       <c r="D3" t="s">
-        <v>425</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>426</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>427</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>190</v>
+        <v>520</v>
       </c>
       <c r="H3" t="s">
         <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>155</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>428</v>
+        <v>50</v>
       </c>
       <c r="K3" t="s">
         <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>170</v>
+        <v>51</v>
       </c>
       <c r="M3" t="s">
-        <v>430</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>431</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>432</v>
+        <v>54</v>
       </c>
       <c r="P3" t="s">
-        <v>412</v>
+        <v>448</v>
       </c>
       <c r="Q3" t="s">
         <v>40</v>
       </c>
       <c r="R3" t="s">
-        <v>429</v>
+        <v>55</v>
       </c>
       <c r="S3" t="s">
-        <v>437</v>
+        <v>56</v>
       </c>
       <c r="T3" t="s">
-        <v>433</v>
+        <v>57</v>
       </c>
       <c r="U3" t="s">
         <v>39</v>
       </c>
       <c r="V3" t="s">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="W3" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="X3" t="s">
         <v>58</v>
@@ -3930,8 +3930,8 @@
       <c r="AA3" t="s">
         <v>61</v>
       </c>
-      <c r="AB3" t="s">
-        <v>580</v>
+      <c r="AB3" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC3">
         <v>1.5</v>
@@ -3940,81 +3940,81 @@
         <v>55</v>
       </c>
       <c r="AE3" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF3" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>62</v>
       </c>
       <c r="C4">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>201</v>
+        <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>520</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>202</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>203</v>
+        <v>67</v>
       </c>
       <c r="K4" t="s">
         <v>40</v>
       </c>
       <c r="L4" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
       <c r="M4" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
       <c r="N4" t="s">
-        <v>208</v>
+        <v>390</v>
       </c>
       <c r="O4" t="s">
-        <v>389</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="Q4" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="R4" t="s">
-        <v>209</v>
+        <v>55</v>
       </c>
       <c r="S4" t="s">
-        <v>204</v>
+        <v>72</v>
       </c>
       <c r="T4" t="s">
-        <v>210</v>
+        <v>57</v>
       </c>
       <c r="U4" t="s">
         <v>39</v>
       </c>
       <c r="V4" t="s">
-        <v>211</v>
+        <v>40</v>
       </c>
       <c r="W4" s="20" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="X4" t="s">
         <v>73</v>
@@ -4028,8 +4028,8 @@
       <c r="AA4" t="s">
         <v>76</v>
       </c>
-      <c r="AB4" t="s">
-        <v>580</v>
+      <c r="AB4" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC4">
         <v>3</v>
@@ -4038,33 +4038,33 @@
         <v>55</v>
       </c>
       <c r="AE4" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF4" s="20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="C5">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>521</v>
       </c>
       <c r="H5" t="s">
         <v>95</v>
@@ -4073,46 +4073,46 @@
         <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>284</v>
       </c>
       <c r="L5" t="s">
         <v>89</v>
       </c>
       <c r="M5" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="N5" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="O5" t="s">
-        <v>388</v>
+        <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q5" t="s">
         <v>40</v>
       </c>
       <c r="R5" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="S5" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="T5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="U5" t="s">
-        <v>560</v>
+        <v>39</v>
       </c>
       <c r="V5" t="s">
         <v>40</v>
       </c>
       <c r="W5" s="20" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="X5" t="s">
         <v>92</v>
@@ -4126,91 +4126,91 @@
       <c r="AA5" t="s">
         <v>93</v>
       </c>
-      <c r="AB5" t="s">
-        <v>580</v>
+      <c r="AB5" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AE5" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AF5" s="20" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>121</v>
       </c>
       <c r="C6">
         <v>2014</v>
       </c>
       <c r="D6" t="s">
-        <v>277</v>
+        <v>101</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>279</v>
+        <v>105</v>
       </c>
       <c r="G6" t="s">
-        <v>525</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
         <v>95</v>
       </c>
       <c r="I6" t="s">
-        <v>533</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>280</v>
+        <v>125</v>
       </c>
       <c r="K6" t="s">
-        <v>284</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
         <v>89</v>
       </c>
       <c r="M6" t="s">
-        <v>286</v>
+        <v>126</v>
       </c>
       <c r="N6" t="s">
-        <v>285</v>
+        <v>127</v>
       </c>
       <c r="O6" t="s">
-        <v>545</v>
+        <v>388</v>
       </c>
       <c r="P6" t="s">
-        <v>549</v>
+        <v>412</v>
       </c>
       <c r="Q6" t="s">
         <v>40</v>
       </c>
       <c r="R6" t="s">
-        <v>287</v>
+        <v>128</v>
       </c>
       <c r="S6" t="s">
-        <v>281</v>
+        <v>129</v>
       </c>
       <c r="T6" t="s">
-        <v>288</v>
+        <v>115</v>
       </c>
       <c r="U6" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="V6" t="s">
         <v>40</v>
       </c>
       <c r="W6" s="20" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="X6" t="s">
         <v>117</v>
@@ -4224,40 +4224,40 @@
       <c r="AA6" t="s">
         <v>131</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AB6" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC6">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AE6" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AF6" s="20" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C7">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="G7" t="s">
         <v>522</v>
@@ -4266,40 +4266,40 @@
         <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>530</v>
       </c>
       <c r="J7" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="K7" t="s">
-        <v>284</v>
+        <v>135</v>
       </c>
       <c r="L7" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="M7" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="N7" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="O7" t="s">
-        <v>40</v>
+        <v>257</v>
       </c>
       <c r="P7" t="s">
-        <v>40</v>
+        <v>412</v>
       </c>
       <c r="Q7" t="s">
         <v>40</v>
       </c>
       <c r="R7" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="S7" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="T7" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="U7" t="s">
         <v>39</v>
@@ -4308,7 +4308,7 @@
         <v>40</v>
       </c>
       <c r="W7" s="20" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="X7" t="s">
         <v>140</v>
@@ -4322,82 +4322,82 @@
       <c r="AA7" t="s">
         <v>143</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AB7" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC7">
         <v>30</v>
       </c>
       <c r="AD7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AE7" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF7" s="20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
       <c r="C8">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D8" t="s">
-        <v>293</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>294</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>295</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
-        <v>526</v>
+        <v>144</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
+        <v>519</v>
       </c>
       <c r="I8" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="J8" t="s">
-        <v>296</v>
+        <v>145</v>
       </c>
       <c r="K8" t="s">
         <v>40</v>
       </c>
       <c r="L8" t="s">
-        <v>297</v>
+        <v>110</v>
       </c>
       <c r="M8" t="s">
-        <v>304</v>
+        <v>146</v>
       </c>
       <c r="N8" t="s">
-        <v>302</v>
+        <v>112</v>
       </c>
       <c r="O8" t="s">
-        <v>40</v>
+        <v>412</v>
       </c>
       <c r="P8" t="s">
-        <v>40</v>
+        <v>412</v>
       </c>
       <c r="Q8" t="s">
         <v>40</v>
       </c>
       <c r="R8" t="s">
-        <v>303</v>
+        <v>147</v>
       </c>
       <c r="S8" t="s">
-        <v>298</v>
+        <v>114</v>
       </c>
       <c r="T8" t="s">
-        <v>299</v>
+        <v>148</v>
       </c>
       <c r="U8" t="s">
         <v>39</v>
@@ -4406,7 +4406,7 @@
         <v>40</v>
       </c>
       <c r="W8" s="20" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="X8" t="s">
         <v>118</v>
@@ -4420,64 +4420,64 @@
       <c r="AA8" t="s">
         <v>150</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AB8" s="20" t="s">
         <v>516</v>
       </c>
       <c r="AC8">
         <v>4</v>
       </c>
       <c r="AD8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AE8" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF8" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="C9">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="G9" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="H9" t="s">
         <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="L9" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="M9" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="N9" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="O9" t="s">
         <v>40</v>
@@ -4486,25 +4486,25 @@
         <v>40</v>
       </c>
       <c r="Q9" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="R9" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="S9" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="T9" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="U9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="V9" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="W9" s="20" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="X9" t="s">
         <v>179</v>
@@ -4518,91 +4518,91 @@
       <c r="AA9" t="s">
         <v>181</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AB9" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC9">
         <v>0</v>
       </c>
       <c r="AD9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AE9" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AF9" s="20" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>124</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
-        <v>249</v>
+        <v>152</v>
       </c>
       <c r="F10" t="s">
-        <v>255</v>
+        <v>107</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
         <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>534</v>
+        <v>155</v>
       </c>
       <c r="J10" t="s">
-        <v>256</v>
+        <v>154</v>
       </c>
       <c r="K10" t="s">
         <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M10" t="s">
-        <v>250</v>
+        <v>157</v>
       </c>
       <c r="N10" t="s">
-        <v>251</v>
+        <v>156</v>
       </c>
       <c r="O10" t="s">
-        <v>257</v>
+        <v>40</v>
       </c>
       <c r="P10" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q10" t="s">
         <v>40</v>
       </c>
       <c r="R10" t="s">
-        <v>258</v>
+        <v>113</v>
       </c>
       <c r="S10" t="s">
-        <v>252</v>
+        <v>159</v>
       </c>
       <c r="T10" t="s">
-        <v>253</v>
+        <v>158</v>
       </c>
       <c r="U10" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="V10" t="s">
         <v>40</v>
       </c>
       <c r="W10" s="20" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="X10" t="s">
         <v>162</v>
@@ -4616,91 +4616,91 @@
       <c r="AA10" t="s">
         <v>163</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AB10" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC10">
         <v>6</v>
       </c>
       <c r="AD10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AE10" s="20" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AF10" s="20" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C11">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="D11" t="s">
-        <v>350</v>
+        <v>184</v>
       </c>
       <c r="E11" t="s">
-        <v>351</v>
+        <v>185</v>
       </c>
       <c r="F11" t="s">
-        <v>354</v>
+        <v>186</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="H11" t="s">
-        <v>95</v>
+        <v>460</v>
       </c>
       <c r="I11" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="J11" t="s">
-        <v>355</v>
+        <v>531</v>
       </c>
       <c r="K11" t="s">
+        <v>191</v>
+      </c>
+      <c r="L11" t="s">
+        <v>170</v>
+      </c>
+      <c r="M11" t="s">
+        <v>194</v>
+      </c>
+      <c r="N11" t="s">
+        <v>187</v>
+      </c>
+      <c r="O11" t="s">
         <v>40</v>
       </c>
-      <c r="L11" t="s">
-        <v>110</v>
-      </c>
-      <c r="M11" t="s">
-        <v>356</v>
-      </c>
-      <c r="N11" t="s">
-        <v>352</v>
-      </c>
-      <c r="O11" t="s">
-        <v>70</v>
-      </c>
       <c r="P11" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q11" t="s">
         <v>40</v>
       </c>
       <c r="R11" t="s">
-        <v>357</v>
+        <v>192</v>
       </c>
       <c r="S11" t="s">
-        <v>358</v>
+        <v>188</v>
       </c>
       <c r="T11" t="s">
-        <v>359</v>
+        <v>193</v>
       </c>
       <c r="U11" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="V11" t="s">
-        <v>40</v>
+        <v>189</v>
       </c>
       <c r="W11" s="20" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="X11" t="s">
         <v>195</v>
@@ -4714,7 +4714,7 @@
       <c r="AA11" t="s">
         <v>197</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AB11" s="20" t="s">
         <v>517</v>
       </c>
       <c r="AC11">
@@ -4724,42 +4724,42 @@
         <v>55</v>
       </c>
       <c r="AE11" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF11" s="20" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>198</v>
       </c>
       <c r="C12">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="D12" t="s">
-        <v>376</v>
+        <v>199</v>
       </c>
       <c r="E12" t="s">
-        <v>377</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>378</v>
+        <v>201</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>519</v>
       </c>
       <c r="I12" t="s">
-        <v>541</v>
+        <v>202</v>
       </c>
       <c r="J12" t="s">
-        <v>379</v>
+        <v>203</v>
       </c>
       <c r="K12" t="s">
         <v>40</v>
@@ -4768,10 +4768,10 @@
         <v>170</v>
       </c>
       <c r="M12" t="s">
-        <v>380</v>
+        <v>207</v>
       </c>
       <c r="N12" t="s">
-        <v>381</v>
+        <v>208</v>
       </c>
       <c r="O12" t="s">
         <v>389</v>
@@ -4783,22 +4783,22 @@
         <v>40</v>
       </c>
       <c r="R12" t="s">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="S12" t="s">
-        <v>382</v>
+        <v>204</v>
       </c>
       <c r="T12" t="s">
-        <v>383</v>
+        <v>210</v>
       </c>
       <c r="U12" t="s">
         <v>39</v>
       </c>
       <c r="V12" t="s">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="W12" s="20" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="X12" t="s">
         <v>205</v>
@@ -4812,52 +4812,52 @@
       <c r="AA12" t="s">
         <v>212</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AB12" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC12">
         <v>25</v>
       </c>
       <c r="AD12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE12" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF12" s="20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>362</v>
+        <v>216</v>
       </c>
       <c r="C13">
-        <v>2017</v>
+        <v>2024</v>
       </c>
       <c r="D13" t="s">
-        <v>363</v>
+        <v>217</v>
       </c>
       <c r="E13" t="s">
-        <v>365</v>
+        <v>218</v>
       </c>
       <c r="F13" t="s">
-        <v>366</v>
+        <v>225</v>
       </c>
       <c r="G13" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>367</v>
+        <v>95</v>
       </c>
       <c r="I13" t="s">
-        <v>155</v>
+        <v>219</v>
       </c>
       <c r="J13" t="s">
-        <v>368</v>
+        <v>220</v>
       </c>
       <c r="K13" t="s">
         <v>40</v>
@@ -4866,28 +4866,28 @@
         <v>170</v>
       </c>
       <c r="M13" t="s">
-        <v>369</v>
+        <v>221</v>
       </c>
       <c r="N13" t="s">
-        <v>370</v>
+        <v>226</v>
       </c>
       <c r="O13" t="s">
-        <v>257</v>
+        <v>448</v>
       </c>
       <c r="P13" t="s">
-        <v>412</v>
+        <v>448</v>
       </c>
       <c r="Q13" t="s">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="R13" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
       <c r="S13" t="s">
-        <v>371</v>
+        <v>222</v>
       </c>
       <c r="T13" t="s">
-        <v>372</v>
+        <v>223</v>
       </c>
       <c r="U13" t="s">
         <v>39</v>
@@ -4896,7 +4896,7 @@
         <v>40</v>
       </c>
       <c r="W13" s="20" t="s">
-        <v>562</v>
+        <v>576</v>
       </c>
       <c r="X13" t="s">
         <v>229</v>
@@ -4910,7 +4910,7 @@
       <c r="AA13" t="s">
         <v>231</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AB13" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC13">
@@ -4920,81 +4920,81 @@
         <v>55</v>
       </c>
       <c r="AE13" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF13" s="20" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>232</v>
       </c>
       <c r="C14">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D14" t="s">
-        <v>391</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
-        <v>392</v>
+        <v>234</v>
       </c>
       <c r="F14" t="s">
-        <v>393</v>
+        <v>235</v>
       </c>
       <c r="G14" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H14" t="s">
-        <v>95</v>
+        <v>460</v>
       </c>
       <c r="I14" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="J14" t="s">
-        <v>394</v>
+        <v>236</v>
       </c>
       <c r="K14" t="s">
         <v>40</v>
       </c>
       <c r="L14" t="s">
-        <v>89</v>
+        <v>238</v>
       </c>
       <c r="M14" t="s">
-        <v>399</v>
+        <v>240</v>
       </c>
       <c r="N14" t="s">
-        <v>395</v>
+        <v>237</v>
       </c>
       <c r="O14" t="s">
-        <v>546</v>
+        <v>40</v>
       </c>
       <c r="P14" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q14" t="s">
         <v>40</v>
       </c>
       <c r="R14" t="s">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="S14" t="s">
-        <v>401</v>
+        <v>241</v>
       </c>
       <c r="T14" t="s">
-        <v>396</v>
+        <v>57</v>
       </c>
       <c r="U14" t="s">
         <v>39</v>
       </c>
       <c r="V14" t="s">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="W14" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="X14" t="s">
         <v>243</v>
@@ -5008,91 +5008,91 @@
       <c r="AA14" t="s">
         <v>239</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AB14" s="20" t="s">
         <v>516</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE14" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF14" s="20" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="C15">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D15" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="E15" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F15" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="G15" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>460</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
         <v>533</v>
       </c>
       <c r="J15" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="K15" t="s">
         <v>40</v>
       </c>
       <c r="L15" t="s">
-        <v>238</v>
+        <v>110</v>
       </c>
       <c r="M15" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="N15" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="O15" t="s">
-        <v>40</v>
+        <v>257</v>
       </c>
       <c r="P15" t="s">
-        <v>40</v>
+        <v>412</v>
       </c>
       <c r="Q15" t="s">
         <v>40</v>
       </c>
       <c r="R15" t="s">
-        <v>40</v>
+        <v>258</v>
       </c>
       <c r="S15" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="T15" t="s">
-        <v>57</v>
+        <v>253</v>
       </c>
       <c r="U15" t="s">
         <v>39</v>
       </c>
       <c r="V15" t="s">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="W15" s="20" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="X15" t="s">
         <v>254</v>
@@ -5106,85 +5106,85 @@
       <c r="AA15" t="s">
         <v>261</v>
       </c>
-      <c r="AB15" t="s">
-        <v>580</v>
+      <c r="AB15" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC15">
         <v>18</v>
       </c>
       <c r="AD15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AE15" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AF15" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C16">
-        <v>2019</v>
+        <v>2024</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>262</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>271</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>263</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>523</v>
       </c>
       <c r="H16" t="s">
         <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>29</v>
+        <v>534</v>
       </c>
       <c r="J16" t="s">
-        <v>67</v>
+        <v>272</v>
       </c>
       <c r="K16" t="s">
         <v>40</v>
       </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>264</v>
       </c>
       <c r="M16" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="N16" t="s">
-        <v>390</v>
+        <v>266</v>
       </c>
       <c r="O16" t="s">
-        <v>70</v>
+        <v>448</v>
       </c>
       <c r="P16" t="s">
-        <v>412</v>
+        <v>448</v>
       </c>
       <c r="Q16" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="R16" t="s">
-        <v>55</v>
+        <v>267</v>
       </c>
       <c r="S16" t="s">
-        <v>72</v>
+        <v>268</v>
       </c>
       <c r="T16" t="s">
-        <v>57</v>
+        <v>269</v>
       </c>
       <c r="U16" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="V16" t="s">
         <v>40</v>
@@ -5204,8 +5204,8 @@
       <c r="AA16" t="s">
         <v>270</v>
       </c>
-      <c r="AB16" t="s">
-        <v>580</v>
+      <c r="AB16" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC16">
         <v>15</v>
@@ -5214,81 +5214,81 @@
         <v>55</v>
       </c>
       <c r="AE16" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF16" s="20" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="17" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>276</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>277</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
+        <v>278</v>
       </c>
       <c r="F17" t="s">
-        <v>166</v>
+        <v>279</v>
       </c>
       <c r="G17" t="s">
-        <v>172</v>
+        <v>524</v>
       </c>
       <c r="H17" t="s">
         <v>95</v>
       </c>
       <c r="I17" t="s">
-        <v>173</v>
+        <v>532</v>
       </c>
       <c r="J17" t="s">
-        <v>167</v>
+        <v>280</v>
       </c>
       <c r="K17" t="s">
-        <v>169</v>
+        <v>284</v>
       </c>
       <c r="L17" t="s">
-        <v>170</v>
+        <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>171</v>
+        <v>286</v>
       </c>
       <c r="N17" t="s">
-        <v>174</v>
+        <v>285</v>
       </c>
       <c r="O17" t="s">
+        <v>544</v>
+      </c>
+      <c r="P17" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q17" t="s">
         <v>40</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
+        <v>287</v>
+      </c>
+      <c r="S17" t="s">
+        <v>281</v>
+      </c>
+      <c r="T17" t="s">
+        <v>288</v>
+      </c>
+      <c r="U17" t="s">
+        <v>39</v>
+      </c>
+      <c r="V17" t="s">
         <v>40</v>
       </c>
-      <c r="Q17" t="s">
-        <v>175</v>
-      </c>
-      <c r="R17" t="s">
-        <v>176</v>
-      </c>
-      <c r="S17" t="s">
-        <v>182</v>
-      </c>
-      <c r="T17" t="s">
-        <v>177</v>
-      </c>
-      <c r="U17" t="s">
-        <v>560</v>
-      </c>
-      <c r="V17" t="s">
-        <v>178</v>
-      </c>
       <c r="W17" s="20" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="X17" t="s">
         <v>289</v>
@@ -5302,91 +5302,91 @@
       <c r="AA17" t="s">
         <v>283</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AB17" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC17">
         <v>0</v>
       </c>
       <c r="AD17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE17" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AF17" s="20" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C18">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="D18" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="E18" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="F18" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="G18" t="s">
-        <v>206</v>
+        <v>525</v>
       </c>
       <c r="H18" t="s">
-        <v>460</v>
+        <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="J18" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="K18" t="s">
         <v>40</v>
       </c>
       <c r="L18" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="M18" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="N18" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="O18" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="P18" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q18" t="s">
         <v>40</v>
       </c>
       <c r="R18" t="s">
+        <v>303</v>
+      </c>
+      <c r="S18" t="s">
+        <v>298</v>
+      </c>
+      <c r="T18" t="s">
+        <v>299</v>
+      </c>
+      <c r="U18" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" t="s">
         <v>40</v>
       </c>
-      <c r="S18" t="s">
-        <v>323</v>
-      </c>
-      <c r="T18" t="s">
-        <v>334</v>
-      </c>
-      <c r="U18" t="s">
-        <v>560</v>
-      </c>
-      <c r="V18" t="s">
-        <v>324</v>
-      </c>
       <c r="W18" s="20" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="X18" t="s">
         <v>300</v>
@@ -5400,91 +5400,91 @@
       <c r="AA18" t="s">
         <v>301</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AB18" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC18">
         <v>3</v>
       </c>
       <c r="AD18" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AE18" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AF18" s="20" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>307</v>
       </c>
       <c r="C19">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>308</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>326</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>309</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
       <c r="H19" t="s">
-        <v>520</v>
+        <v>95</v>
       </c>
       <c r="I19" t="s">
-        <v>530</v>
+        <v>539</v>
       </c>
       <c r="J19" t="s">
-        <v>145</v>
+        <v>327</v>
       </c>
       <c r="K19" t="s">
+        <v>330</v>
+      </c>
+      <c r="L19" t="s">
+        <v>310</v>
+      </c>
+      <c r="M19" t="s">
+        <v>328</v>
+      </c>
+      <c r="N19" t="s">
+        <v>311</v>
+      </c>
+      <c r="O19" t="s">
         <v>40</v>
       </c>
-      <c r="L19" t="s">
-        <v>110</v>
-      </c>
-      <c r="M19" t="s">
-        <v>146</v>
-      </c>
-      <c r="N19" t="s">
-        <v>112</v>
-      </c>
-      <c r="O19" t="s">
-        <v>412</v>
-      </c>
       <c r="P19" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q19" t="s">
+        <v>329</v>
+      </c>
+      <c r="R19" t="s">
         <v>40</v>
       </c>
-      <c r="R19" t="s">
-        <v>147</v>
-      </c>
       <c r="S19" t="s">
-        <v>114</v>
+        <v>331</v>
       </c>
       <c r="T19" t="s">
-        <v>148</v>
+        <v>312</v>
       </c>
       <c r="U19" t="s">
-        <v>555</v>
+        <v>39</v>
       </c>
       <c r="V19" t="s">
-        <v>40</v>
+        <v>282</v>
       </c>
       <c r="W19" s="20" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="X19" t="s">
         <v>313</v>
@@ -5498,43 +5498,43 @@
       <c r="AA19" t="s">
         <v>332</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AB19" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC19">
         <v>0</v>
       </c>
       <c r="AD19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE19" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF19" s="20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>404</v>
+        <v>81</v>
       </c>
       <c r="C20">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="D20" t="s">
-        <v>405</v>
+        <v>338</v>
       </c>
       <c r="E20" t="s">
-        <v>406</v>
+        <v>339</v>
       </c>
       <c r="F20" t="s">
-        <v>409</v>
+        <v>340</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>526</v>
       </c>
       <c r="H20" t="s">
         <v>95</v>
@@ -5543,7 +5543,7 @@
         <v>536</v>
       </c>
       <c r="J20" t="s">
-        <v>407</v>
+        <v>341</v>
       </c>
       <c r="K20" t="s">
         <v>40</v>
@@ -5552,37 +5552,37 @@
         <v>170</v>
       </c>
       <c r="M20" t="s">
-        <v>410</v>
+        <v>347</v>
       </c>
       <c r="N20" t="s">
-        <v>411</v>
+        <v>342</v>
       </c>
       <c r="O20" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="P20" t="s">
-        <v>412</v>
+        <v>40</v>
       </c>
       <c r="Q20" t="s">
         <v>40</v>
       </c>
       <c r="R20" t="s">
-        <v>408</v>
+        <v>40</v>
       </c>
       <c r="S20" t="s">
-        <v>413</v>
+        <v>343</v>
       </c>
       <c r="T20" t="s">
-        <v>414</v>
+        <v>344</v>
       </c>
       <c r="U20" t="s">
-        <v>560</v>
+        <v>39</v>
       </c>
       <c r="V20" t="s">
         <v>183</v>
       </c>
       <c r="W20" s="20" t="s">
-        <v>562</v>
+        <v>577</v>
       </c>
       <c r="X20" t="s">
         <v>349</v>
@@ -5596,91 +5596,91 @@
       <c r="AA20" t="s">
         <v>346</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AB20" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC20">
         <v>14</v>
       </c>
       <c r="AD20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE20" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF20" s="20" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>471</v>
+        <v>316</v>
       </c>
       <c r="C21">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D21" t="s">
-        <v>472</v>
+        <v>317</v>
       </c>
       <c r="E21" t="s">
-        <v>473</v>
+        <v>318</v>
       </c>
       <c r="F21" t="s">
-        <v>474</v>
+        <v>319</v>
       </c>
       <c r="G21" t="s">
-        <v>528</v>
+        <v>206</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>460</v>
       </c>
       <c r="I21" t="s">
-        <v>155</v>
+        <v>538</v>
       </c>
       <c r="J21" t="s">
-        <v>476</v>
+        <v>320</v>
       </c>
       <c r="K21" t="s">
         <v>40</v>
       </c>
       <c r="L21" t="s">
-        <v>110</v>
+        <v>321</v>
       </c>
       <c r="M21" t="s">
-        <v>478</v>
+        <v>333</v>
       </c>
       <c r="N21" t="s">
-        <v>477</v>
+        <v>322</v>
       </c>
       <c r="O21" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="P21" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="Q21" t="s">
         <v>40</v>
       </c>
       <c r="R21" t="s">
-        <v>479</v>
+        <v>40</v>
       </c>
       <c r="S21" t="s">
-        <v>480</v>
+        <v>323</v>
       </c>
       <c r="T21" t="s">
-        <v>475</v>
+        <v>334</v>
       </c>
       <c r="U21" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="V21" t="s">
-        <v>183</v>
+        <v>324</v>
       </c>
       <c r="W21" s="20" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="X21" t="s">
         <v>336</v>
@@ -5694,67 +5694,67 @@
       <c r="AA21" t="s">
         <v>337</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AB21" s="20" t="s">
         <v>518</v>
       </c>
       <c r="AC21">
         <v>1</v>
       </c>
       <c r="AD21" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE21" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF21" s="20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="C22">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>350</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>351</v>
       </c>
       <c r="F22" t="s">
-        <v>134</v>
+        <v>354</v>
       </c>
       <c r="G22" t="s">
-        <v>523</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
         <v>95</v>
       </c>
       <c r="I22" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="J22" t="s">
-        <v>108</v>
+        <v>355</v>
       </c>
       <c r="K22" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="L22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M22" t="s">
-        <v>138</v>
+        <v>356</v>
       </c>
       <c r="N22" t="s">
-        <v>137</v>
+        <v>352</v>
       </c>
       <c r="O22" t="s">
-        <v>257</v>
+        <v>70</v>
       </c>
       <c r="P22" t="s">
         <v>412</v>
@@ -5763,13 +5763,13 @@
         <v>40</v>
       </c>
       <c r="R22" t="s">
-        <v>139</v>
+        <v>357</v>
       </c>
       <c r="S22" t="s">
-        <v>136</v>
+        <v>358</v>
       </c>
       <c r="T22" t="s">
-        <v>116</v>
+        <v>359</v>
       </c>
       <c r="U22" t="s">
         <v>39</v>
@@ -5778,7 +5778,7 @@
         <v>40</v>
       </c>
       <c r="W22" s="20" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="X22" t="s">
         <v>360</v>
@@ -5789,43 +5789,43 @@
       <c r="Z22" t="s">
         <v>361</v>
       </c>
-      <c r="AB22" t="s">
-        <v>580</v>
+      <c r="AB22" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC22">
         <v>13</v>
       </c>
       <c r="AD22" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AE22" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AF22" s="20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>307</v>
+        <v>83</v>
       </c>
       <c r="C23">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="D23" t="s">
-        <v>308</v>
+        <v>376</v>
       </c>
       <c r="E23" t="s">
-        <v>326</v>
+        <v>377</v>
       </c>
       <c r="F23" t="s">
-        <v>309</v>
+        <v>378</v>
       </c>
       <c r="G23" t="s">
-        <v>206</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
         <v>95</v>
@@ -5834,46 +5834,46 @@
         <v>540</v>
       </c>
       <c r="J23" t="s">
-        <v>327</v>
+        <v>379</v>
       </c>
       <c r="K23" t="s">
-        <v>330</v>
+        <v>40</v>
       </c>
       <c r="L23" t="s">
-        <v>310</v>
+        <v>170</v>
       </c>
       <c r="M23" t="s">
-        <v>328</v>
+        <v>380</v>
       </c>
       <c r="N23" t="s">
-        <v>311</v>
+        <v>381</v>
       </c>
       <c r="O23" t="s">
+        <v>389</v>
+      </c>
+      <c r="P23" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q23" t="s">
         <v>40</v>
-      </c>
-      <c r="P23" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>329</v>
       </c>
       <c r="R23" t="s">
         <v>40</v>
       </c>
       <c r="S23" t="s">
-        <v>331</v>
+        <v>382</v>
       </c>
       <c r="T23" t="s">
-        <v>312</v>
+        <v>383</v>
       </c>
       <c r="U23" t="s">
         <v>39</v>
       </c>
       <c r="V23" t="s">
-        <v>282</v>
+        <v>40</v>
       </c>
       <c r="W23" s="20" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="X23" t="s">
         <v>385</v>
@@ -5887,91 +5887,91 @@
       <c r="AA23" t="s">
         <v>387</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AB23" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC23">
         <v>12</v>
       </c>
       <c r="AD23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AE23" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF23" s="20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="24" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>453</v>
+        <v>362</v>
       </c>
       <c r="C24">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="D24" t="s">
-        <v>454</v>
+        <v>363</v>
       </c>
       <c r="E24" t="s">
-        <v>455</v>
+        <v>365</v>
       </c>
       <c r="F24" t="s">
-        <v>456</v>
+        <v>366</v>
       </c>
       <c r="G24" t="s">
-        <v>459</v>
+        <v>190</v>
       </c>
       <c r="H24" t="s">
-        <v>460</v>
+        <v>367</v>
       </c>
       <c r="I24" t="s">
-        <v>543</v>
+        <v>155</v>
       </c>
       <c r="J24" t="s">
-        <v>461</v>
+        <v>368</v>
       </c>
       <c r="K24" t="s">
         <v>40</v>
       </c>
       <c r="L24" t="s">
-        <v>457</v>
+        <v>170</v>
       </c>
       <c r="M24" t="s">
-        <v>465</v>
+        <v>369</v>
       </c>
       <c r="N24" t="s">
-        <v>466</v>
+        <v>370</v>
       </c>
       <c r="O24" t="s">
-        <v>448</v>
+        <v>257</v>
       </c>
       <c r="P24" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="Q24" t="s">
         <v>40</v>
       </c>
       <c r="R24" t="s">
-        <v>464</v>
+        <v>55</v>
       </c>
       <c r="S24" t="s">
-        <v>462</v>
+        <v>371</v>
       </c>
       <c r="T24" t="s">
-        <v>458</v>
+        <v>372</v>
       </c>
       <c r="U24" t="s">
         <v>39</v>
       </c>
       <c r="V24" t="s">
-        <v>463</v>
+        <v>40</v>
       </c>
       <c r="W24" s="20" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="X24" t="s">
         <v>364</v>
@@ -5985,8 +5985,8 @@
       <c r="AA24" t="s">
         <v>375</v>
       </c>
-      <c r="AB24" t="s">
-        <v>580</v>
+      <c r="AB24" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC24">
         <v>6</v>
@@ -5995,72 +5995,72 @@
         <v>55</v>
       </c>
       <c r="AE24" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF24" s="20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C25">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>391</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>392</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>393</v>
       </c>
       <c r="G25" t="s">
-        <v>529</v>
+        <v>206</v>
       </c>
       <c r="H25" t="s">
         <v>95</v>
       </c>
       <c r="I25" t="s">
-        <v>29</v>
+        <v>529</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>394</v>
       </c>
       <c r="K25" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L25" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="M25" t="s">
-        <v>33</v>
+        <v>399</v>
       </c>
       <c r="N25" t="s">
-        <v>34</v>
+        <v>395</v>
       </c>
       <c r="O25" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P25" t="s">
         <v>412</v>
       </c>
       <c r="Q25" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R25" t="s">
-        <v>36</v>
+        <v>400</v>
       </c>
       <c r="S25" t="s">
-        <v>37</v>
+        <v>401</v>
       </c>
       <c r="T25" t="s">
-        <v>38</v>
+        <v>396</v>
       </c>
       <c r="U25" t="s">
         <v>39</v>
@@ -6069,7 +6069,7 @@
         <v>40</v>
       </c>
       <c r="W25" s="20" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="X25" t="s">
         <v>402</v>
@@ -6083,52 +6083,52 @@
       <c r="AA25" t="s">
         <v>398</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AB25" s="20" t="s">
         <v>515</v>
       </c>
       <c r="AC25">
         <v>4</v>
       </c>
       <c r="AD25" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AE25" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF25" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>439</v>
+        <v>404</v>
       </c>
       <c r="C26">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D26" t="s">
-        <v>440</v>
+        <v>405</v>
       </c>
       <c r="E26" t="s">
-        <v>441</v>
+        <v>406</v>
       </c>
       <c r="F26" t="s">
-        <v>442</v>
+        <v>409</v>
       </c>
       <c r="G26" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
       <c r="H26" t="s">
         <v>95</v>
       </c>
       <c r="I26" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="J26" t="s">
-        <v>444</v>
+        <v>407</v>
       </c>
       <c r="K26" t="s">
         <v>40</v>
@@ -6137,37 +6137,37 @@
         <v>170</v>
       </c>
       <c r="M26" t="s">
-        <v>446</v>
+        <v>410</v>
       </c>
       <c r="N26" t="s">
-        <v>447</v>
+        <v>411</v>
       </c>
       <c r="O26" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="P26" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="Q26" t="s">
         <v>40</v>
       </c>
       <c r="R26" t="s">
-        <v>445</v>
+        <v>408</v>
       </c>
       <c r="S26" t="s">
-        <v>449</v>
+        <v>413</v>
       </c>
       <c r="T26" t="s">
-        <v>443</v>
+        <v>414</v>
       </c>
       <c r="U26" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="V26" t="s">
         <v>183</v>
       </c>
       <c r="W26" s="20" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="X26" t="s">
         <v>415</v>
@@ -6181,91 +6181,91 @@
       <c r="AA26" t="s">
         <v>416</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AB26" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC26">
         <v>3</v>
       </c>
       <c r="AD26" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AE26" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AF26" s="20" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C27">
-        <v>2024</v>
+        <v>2007</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>425</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>426</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>427</v>
       </c>
       <c r="G27" t="s">
-        <v>521</v>
+        <v>190</v>
       </c>
       <c r="H27" t="s">
         <v>95</v>
       </c>
       <c r="I27" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="J27" t="s">
-        <v>50</v>
+        <v>428</v>
       </c>
       <c r="K27" t="s">
         <v>40</v>
       </c>
       <c r="L27" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
       <c r="M27" t="s">
-        <v>52</v>
+        <v>430</v>
       </c>
       <c r="N27" t="s">
-        <v>53</v>
+        <v>431</v>
       </c>
       <c r="O27" t="s">
-        <v>54</v>
+        <v>432</v>
       </c>
       <c r="P27" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="Q27" t="s">
         <v>40</v>
       </c>
       <c r="R27" t="s">
-        <v>55</v>
+        <v>429</v>
       </c>
       <c r="S27" t="s">
-        <v>56</v>
+        <v>437</v>
       </c>
       <c r="T27" t="s">
-        <v>57</v>
+        <v>433</v>
       </c>
       <c r="U27" t="s">
         <v>39</v>
       </c>
       <c r="V27" t="s">
-        <v>40</v>
+        <v>183</v>
       </c>
       <c r="W27" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="X27" t="s">
         <v>434</v>
@@ -6279,7 +6279,7 @@
       <c r="AA27" t="s">
         <v>438</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AB27" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AC27">
@@ -6289,42 +6289,42 @@
         <v>55</v>
       </c>
       <c r="AE27" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF27" s="20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>439</v>
       </c>
       <c r="C28">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>440</v>
       </c>
       <c r="E28" t="s">
-        <v>218</v>
+        <v>441</v>
       </c>
       <c r="F28" t="s">
-        <v>225</v>
+        <v>442</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="H28" t="s">
         <v>95</v>
       </c>
       <c r="I28" t="s">
-        <v>219</v>
+        <v>541</v>
       </c>
       <c r="J28" t="s">
-        <v>220</v>
+        <v>444</v>
       </c>
       <c r="K28" t="s">
         <v>40</v>
@@ -6333,10 +6333,10 @@
         <v>170</v>
       </c>
       <c r="M28" t="s">
-        <v>221</v>
+        <v>446</v>
       </c>
       <c r="N28" t="s">
-        <v>226</v>
+        <v>447</v>
       </c>
       <c r="O28" t="s">
         <v>448</v>
@@ -6345,25 +6345,25 @@
         <v>448</v>
       </c>
       <c r="Q28" t="s">
-        <v>227</v>
+        <v>40</v>
       </c>
       <c r="R28" t="s">
-        <v>228</v>
+        <v>445</v>
       </c>
       <c r="S28" t="s">
-        <v>222</v>
+        <v>449</v>
       </c>
       <c r="T28" t="s">
-        <v>223</v>
+        <v>443</v>
       </c>
       <c r="U28" t="s">
-        <v>555</v>
+        <v>39</v>
       </c>
       <c r="V28" t="s">
-        <v>40</v>
+        <v>183</v>
       </c>
       <c r="W28" s="20" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="X28" t="s">
         <v>450</v>
@@ -6377,64 +6377,64 @@
       <c r="AA28" t="s">
         <v>452</v>
       </c>
-      <c r="AB28" t="s">
-        <v>580</v>
+      <c r="AB28" s="20" t="s">
+        <v>579</v>
       </c>
       <c r="AC28">
         <v>0</v>
       </c>
       <c r="AD28" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AE28" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF28" s="20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>453</v>
       </c>
       <c r="C29">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="D29" t="s">
-        <v>262</v>
+        <v>454</v>
       </c>
       <c r="E29" t="s">
-        <v>271</v>
+        <v>455</v>
       </c>
       <c r="F29" t="s">
-        <v>263</v>
+        <v>456</v>
       </c>
       <c r="G29" t="s">
-        <v>524</v>
+        <v>459</v>
       </c>
       <c r="H29" t="s">
-        <v>95</v>
+        <v>460</v>
       </c>
       <c r="I29" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
       <c r="J29" t="s">
-        <v>272</v>
+        <v>461</v>
       </c>
       <c r="K29" t="s">
         <v>40</v>
       </c>
       <c r="L29" t="s">
-        <v>264</v>
+        <v>457</v>
       </c>
       <c r="M29" t="s">
-        <v>265</v>
+        <v>465</v>
       </c>
       <c r="N29" t="s">
-        <v>266</v>
+        <v>466</v>
       </c>
       <c r="O29" t="s">
         <v>448</v>
@@ -6446,22 +6446,22 @@
         <v>40</v>
       </c>
       <c r="R29" t="s">
-        <v>267</v>
+        <v>464</v>
       </c>
       <c r="S29" t="s">
-        <v>268</v>
+        <v>462</v>
       </c>
       <c r="T29" t="s">
-        <v>269</v>
+        <v>458</v>
       </c>
       <c r="U29" t="s">
-        <v>560</v>
+        <v>39</v>
       </c>
       <c r="V29" t="s">
-        <v>40</v>
+        <v>463</v>
       </c>
       <c r="W29" s="20" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="X29" t="s">
         <v>467</v>
@@ -6475,37 +6475,37 @@
       <c r="AA29" t="s">
         <v>470</v>
       </c>
-      <c r="AB29" t="s">
+      <c r="AB29" s="20" t="s">
         <v>518</v>
       </c>
       <c r="AD29" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AE29" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF29" s="20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>471</v>
       </c>
       <c r="C30">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="D30" t="s">
-        <v>338</v>
+        <v>472</v>
       </c>
       <c r="E30" t="s">
-        <v>339</v>
+        <v>473</v>
       </c>
       <c r="F30" t="s">
-        <v>340</v>
+        <v>474</v>
       </c>
       <c r="G30" t="s">
         <v>527</v>
@@ -6514,49 +6514,49 @@
         <v>95</v>
       </c>
       <c r="I30" t="s">
-        <v>537</v>
+        <v>155</v>
       </c>
       <c r="J30" t="s">
-        <v>341</v>
+        <v>476</v>
       </c>
       <c r="K30" t="s">
         <v>40</v>
       </c>
       <c r="L30" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="M30" t="s">
-        <v>347</v>
+        <v>478</v>
       </c>
       <c r="N30" t="s">
-        <v>342</v>
+        <v>477</v>
       </c>
       <c r="O30" t="s">
-        <v>40</v>
+        <v>448</v>
       </c>
       <c r="P30" t="s">
-        <v>40</v>
+        <v>448</v>
       </c>
       <c r="Q30" t="s">
         <v>40</v>
       </c>
       <c r="R30" t="s">
-        <v>40</v>
+        <v>479</v>
       </c>
       <c r="S30" t="s">
-        <v>343</v>
+        <v>480</v>
       </c>
       <c r="T30" t="s">
-        <v>344</v>
+        <v>475</v>
       </c>
       <c r="U30" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="V30" t="s">
         <v>183</v>
       </c>
       <c r="W30" s="20" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
       <c r="X30" t="s">
         <v>482</v>
@@ -6570,867 +6570,1325 @@
       <c r="AA30" t="s">
         <v>483</v>
       </c>
-      <c r="AB30" t="s">
+      <c r="AB30" s="20" t="s">
         <v>514</v>
       </c>
       <c r="AD30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AE30" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF30" s="20" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="31" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W31" s="20"/>
+      <c r="AB31" s="20"/>
       <c r="AE31" s="20"/>
       <c r="AF31" s="20"/>
     </row>
     <row r="32" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W32" s="20"/>
+      <c r="AB32" s="20"/>
       <c r="AE32" s="20"/>
       <c r="AF32" s="20"/>
     </row>
     <row r="33" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W33" s="20"/>
+      <c r="AB33" s="20"/>
       <c r="AE33" s="20"/>
       <c r="AF33" s="20"/>
     </row>
     <row r="34" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W34" s="20"/>
+      <c r="AB34" s="20"/>
       <c r="AE34" s="20"/>
       <c r="AF34" s="20"/>
     </row>
     <row r="35" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W35" s="20"/>
+      <c r="AB35" s="20"/>
       <c r="AE35" s="20"/>
       <c r="AF35" s="20"/>
     </row>
     <row r="36" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W36" s="20"/>
+      <c r="AB36" s="20"/>
       <c r="AE36" s="20"/>
       <c r="AF36" s="20"/>
     </row>
     <row r="37" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W37" s="20"/>
+      <c r="AB37" s="20"/>
       <c r="AE37" s="20"/>
       <c r="AF37" s="20"/>
     </row>
     <row r="38" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W38" s="20"/>
+      <c r="AB38" s="20"/>
       <c r="AE38" s="20"/>
       <c r="AF38" s="20"/>
     </row>
     <row r="39" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W39" s="20"/>
+      <c r="AB39" s="20"/>
       <c r="AE39" s="20"/>
       <c r="AF39" s="20"/>
     </row>
     <row r="40" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W40" s="20"/>
+      <c r="AB40" s="20"/>
       <c r="AE40" s="20"/>
       <c r="AF40" s="20"/>
     </row>
     <row r="41" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W41" s="20"/>
+      <c r="AB41" s="20"/>
       <c r="AE41" s="20"/>
       <c r="AF41" s="20"/>
     </row>
     <row r="42" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W42" s="20"/>
+      <c r="AB42" s="20"/>
       <c r="AE42" s="20"/>
       <c r="AF42" s="20"/>
     </row>
     <row r="43" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W43" s="20"/>
+      <c r="AB43" s="20"/>
       <c r="AE43" s="20"/>
       <c r="AF43" s="20"/>
     </row>
     <row r="44" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W44" s="20"/>
+      <c r="AB44" s="20"/>
       <c r="AE44" s="20"/>
       <c r="AF44" s="20"/>
     </row>
     <row r="45" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W45" s="20"/>
+      <c r="AB45" s="20"/>
       <c r="AE45" s="20"/>
       <c r="AF45" s="20"/>
     </row>
     <row r="46" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W46" s="20"/>
+      <c r="AB46" s="20"/>
       <c r="AE46" s="20"/>
       <c r="AF46" s="20"/>
     </row>
     <row r="47" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W47" s="20"/>
+      <c r="AB47" s="20"/>
       <c r="AE47" s="20"/>
       <c r="AF47" s="20"/>
     </row>
     <row r="48" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W48" s="20"/>
+      <c r="AB48" s="20"/>
       <c r="AE48" s="20"/>
       <c r="AF48" s="20"/>
     </row>
     <row r="49" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W49" s="20"/>
+      <c r="AB49" s="20"/>
       <c r="AE49" s="20"/>
       <c r="AF49" s="20"/>
     </row>
     <row r="50" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W50" s="20"/>
+      <c r="AB50" s="20"/>
       <c r="AE50" s="20"/>
       <c r="AF50" s="20"/>
     </row>
     <row r="51" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W51" s="20"/>
+      <c r="AB51" s="20"/>
       <c r="AE51" s="20"/>
       <c r="AF51" s="20"/>
     </row>
     <row r="52" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W52" s="20"/>
+      <c r="AB52" s="20"/>
       <c r="AE52" s="20"/>
       <c r="AF52" s="20"/>
     </row>
     <row r="53" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W53" s="20"/>
+      <c r="AB53" s="20"/>
       <c r="AE53" s="20"/>
       <c r="AF53" s="20"/>
     </row>
     <row r="54" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W54" s="20"/>
+      <c r="AB54" s="20"/>
       <c r="AE54" s="20"/>
       <c r="AF54" s="20"/>
     </row>
     <row r="55" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W55" s="20"/>
+      <c r="AB55" s="20"/>
       <c r="AE55" s="20"/>
       <c r="AF55" s="20"/>
     </row>
     <row r="56" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W56" s="20"/>
+      <c r="AB56" s="20"/>
       <c r="AE56" s="20"/>
       <c r="AF56" s="20"/>
     </row>
     <row r="57" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W57" s="20"/>
+      <c r="AB57" s="20"/>
       <c r="AE57" s="20"/>
       <c r="AF57" s="20"/>
     </row>
     <row r="58" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W58" s="20"/>
+      <c r="AB58" s="20"/>
       <c r="AE58" s="20"/>
       <c r="AF58" s="20"/>
     </row>
     <row r="59" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W59" s="20"/>
+      <c r="AB59" s="20"/>
       <c r="AE59" s="20"/>
       <c r="AF59" s="20"/>
     </row>
     <row r="60" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W60" s="20"/>
+      <c r="AB60" s="20"/>
       <c r="AE60" s="20"/>
       <c r="AF60" s="20"/>
     </row>
     <row r="61" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W61" s="20"/>
+      <c r="AB61" s="20"/>
       <c r="AE61" s="20"/>
       <c r="AF61" s="20"/>
     </row>
     <row r="62" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W62" s="20"/>
+      <c r="AB62" s="20"/>
       <c r="AE62" s="20"/>
       <c r="AF62" s="20"/>
     </row>
     <row r="63" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W63" s="20"/>
+      <c r="AB63" s="20"/>
       <c r="AE63" s="20"/>
       <c r="AF63" s="20"/>
     </row>
     <row r="64" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W64" s="20"/>
+      <c r="AB64" s="20"/>
       <c r="AE64" s="20"/>
       <c r="AF64" s="20"/>
     </row>
     <row r="65" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W65" s="20"/>
+      <c r="AB65" s="20"/>
       <c r="AE65" s="20"/>
       <c r="AF65" s="20"/>
     </row>
     <row r="66" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W66" s="20"/>
+      <c r="AB66" s="20"/>
       <c r="AE66" s="20"/>
       <c r="AF66" s="20"/>
     </row>
     <row r="67" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W67" s="20"/>
+      <c r="AB67" s="20"/>
       <c r="AE67" s="20"/>
       <c r="AF67" s="20"/>
     </row>
     <row r="68" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W68" s="20"/>
+      <c r="AB68" s="20"/>
       <c r="AE68" s="20"/>
       <c r="AF68" s="20"/>
     </row>
     <row r="69" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W69" s="20"/>
+      <c r="AB69" s="20"/>
       <c r="AE69" s="20"/>
       <c r="AF69" s="20"/>
     </row>
     <row r="70" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W70" s="20"/>
+      <c r="AB70" s="20"/>
       <c r="AE70" s="20"/>
       <c r="AF70" s="20"/>
     </row>
     <row r="71" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W71" s="20"/>
+      <c r="AB71" s="20"/>
       <c r="AE71" s="20"/>
       <c r="AF71" s="20"/>
     </row>
     <row r="72" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W72" s="20"/>
+      <c r="AB72" s="20"/>
       <c r="AE72" s="20"/>
       <c r="AF72" s="20"/>
     </row>
     <row r="73" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W73" s="20"/>
+      <c r="AB73" s="20"/>
       <c r="AE73" s="20"/>
       <c r="AF73" s="20"/>
     </row>
     <row r="74" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W74" s="20"/>
+      <c r="AB74" s="20"/>
       <c r="AE74" s="20"/>
       <c r="AF74" s="20"/>
     </row>
     <row r="75" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W75" s="20"/>
+      <c r="AB75" s="20"/>
       <c r="AE75" s="20"/>
       <c r="AF75" s="20"/>
     </row>
     <row r="76" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W76" s="20"/>
+      <c r="AB76" s="20"/>
       <c r="AE76" s="20"/>
       <c r="AF76" s="20"/>
     </row>
     <row r="77" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W77" s="20"/>
+      <c r="AB77" s="20"/>
       <c r="AE77" s="20"/>
       <c r="AF77" s="20"/>
     </row>
     <row r="78" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W78" s="20"/>
+      <c r="AB78" s="20"/>
       <c r="AE78" s="20"/>
       <c r="AF78" s="20"/>
     </row>
     <row r="79" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W79" s="20"/>
+      <c r="AB79" s="20"/>
       <c r="AE79" s="20"/>
       <c r="AF79" s="20"/>
     </row>
     <row r="80" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W80" s="20"/>
+      <c r="AB80" s="20"/>
       <c r="AE80" s="20"/>
       <c r="AF80" s="20"/>
     </row>
     <row r="81" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W81" s="20"/>
+      <c r="AB81" s="20"/>
       <c r="AE81" s="20"/>
       <c r="AF81" s="20"/>
     </row>
     <row r="82" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W82" s="20"/>
+      <c r="AB82" s="20"/>
       <c r="AE82" s="20"/>
       <c r="AF82" s="20"/>
     </row>
     <row r="83" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W83" s="20"/>
+      <c r="AB83" s="20"/>
       <c r="AE83" s="20"/>
       <c r="AF83" s="20"/>
     </row>
     <row r="84" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W84" s="20"/>
+      <c r="AB84" s="20"/>
       <c r="AE84" s="20"/>
       <c r="AF84" s="20"/>
     </row>
     <row r="85" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W85" s="20"/>
+      <c r="AB85" s="20"/>
       <c r="AE85" s="20"/>
       <c r="AF85" s="20"/>
     </row>
     <row r="86" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W86" s="20"/>
+      <c r="AB86" s="20"/>
       <c r="AE86" s="20"/>
       <c r="AF86" s="20"/>
     </row>
     <row r="87" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W87" s="20"/>
+      <c r="AB87" s="20"/>
       <c r="AE87" s="20"/>
       <c r="AF87" s="20"/>
     </row>
     <row r="88" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W88" s="20"/>
+      <c r="AB88" s="20"/>
       <c r="AE88" s="20"/>
       <c r="AF88" s="20"/>
     </row>
     <row r="89" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W89" s="20"/>
+      <c r="AB89" s="20"/>
       <c r="AE89" s="20"/>
       <c r="AF89" s="20"/>
     </row>
     <row r="90" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W90" s="20"/>
+      <c r="AB90" s="20"/>
       <c r="AE90" s="20"/>
       <c r="AF90" s="20"/>
     </row>
     <row r="91" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W91" s="20"/>
+      <c r="AB91" s="20"/>
       <c r="AE91" s="20"/>
       <c r="AF91" s="20"/>
     </row>
     <row r="92" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W92" s="20"/>
+      <c r="AB92" s="20"/>
       <c r="AE92" s="20"/>
       <c r="AF92" s="20"/>
     </row>
     <row r="93" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W93" s="20"/>
+      <c r="AB93" s="20"/>
       <c r="AE93" s="20"/>
       <c r="AF93" s="20"/>
     </row>
     <row r="94" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W94" s="20"/>
+      <c r="AB94" s="20"/>
       <c r="AE94" s="20"/>
       <c r="AF94" s="20"/>
     </row>
     <row r="95" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W95" s="20"/>
+      <c r="AB95" s="20"/>
       <c r="AE95" s="20"/>
       <c r="AF95" s="20"/>
     </row>
     <row r="96" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W96" s="20"/>
+      <c r="AB96" s="20"/>
       <c r="AE96" s="20"/>
       <c r="AF96" s="20"/>
     </row>
     <row r="97" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W97" s="20"/>
+      <c r="AB97" s="20"/>
       <c r="AE97" s="20"/>
       <c r="AF97" s="20"/>
     </row>
     <row r="98" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W98" s="20"/>
+      <c r="AB98" s="20"/>
       <c r="AE98" s="20"/>
       <c r="AF98" s="20"/>
     </row>
     <row r="99" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W99" s="20"/>
+      <c r="AB99" s="20"/>
       <c r="AE99" s="20"/>
       <c r="AF99" s="20"/>
     </row>
     <row r="100" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W100" s="20"/>
+      <c r="AB100" s="20"/>
       <c r="AE100" s="20"/>
       <c r="AF100" s="20"/>
     </row>
     <row r="101" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W101" s="20"/>
+      <c r="AB101" s="20"/>
       <c r="AE101" s="20"/>
       <c r="AF101" s="20"/>
     </row>
     <row r="102" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W102" s="20"/>
+      <c r="AB102" s="20"/>
       <c r="AE102" s="20"/>
       <c r="AF102" s="20"/>
     </row>
     <row r="103" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W103" s="20"/>
+      <c r="AB103" s="20"/>
       <c r="AE103" s="20"/>
       <c r="AF103" s="20"/>
     </row>
     <row r="104" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W104" s="20"/>
+      <c r="AB104" s="20"/>
       <c r="AE104" s="20"/>
       <c r="AF104" s="20"/>
     </row>
     <row r="105" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W105" s="20"/>
+      <c r="AB105" s="20"/>
       <c r="AE105" s="20"/>
       <c r="AF105" s="20"/>
     </row>
     <row r="106" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W106" s="20"/>
+      <c r="AB106" s="20"/>
       <c r="AE106" s="20"/>
       <c r="AF106" s="20"/>
     </row>
     <row r="107" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W107" s="20"/>
+      <c r="AB107" s="20"/>
       <c r="AE107" s="20"/>
       <c r="AF107" s="20"/>
     </row>
     <row r="108" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W108" s="20"/>
+      <c r="AB108" s="20"/>
       <c r="AE108" s="20"/>
       <c r="AF108" s="20"/>
     </row>
     <row r="109" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W109" s="20"/>
+      <c r="AB109" s="20"/>
       <c r="AE109" s="20"/>
       <c r="AF109" s="20"/>
     </row>
     <row r="110" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W110" s="20"/>
+      <c r="AB110" s="20"/>
       <c r="AE110" s="20"/>
       <c r="AF110" s="20"/>
     </row>
     <row r="111" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W111" s="20"/>
+      <c r="AB111" s="20"/>
       <c r="AE111" s="20"/>
       <c r="AF111" s="20"/>
     </row>
     <row r="112" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W112" s="20"/>
+      <c r="AB112" s="20"/>
       <c r="AE112" s="20"/>
       <c r="AF112" s="20"/>
     </row>
     <row r="113" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W113" s="20"/>
+      <c r="AB113" s="20"/>
       <c r="AE113" s="20"/>
       <c r="AF113" s="20"/>
     </row>
     <row r="114" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W114" s="20"/>
+      <c r="AB114" s="20"/>
       <c r="AE114" s="20"/>
       <c r="AF114" s="20"/>
     </row>
     <row r="115" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W115" s="20"/>
+      <c r="AB115" s="20"/>
       <c r="AE115" s="20"/>
       <c r="AF115" s="20"/>
     </row>
     <row r="116" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W116" s="20"/>
+      <c r="AB116" s="20"/>
       <c r="AE116" s="20"/>
       <c r="AF116" s="20"/>
     </row>
     <row r="117" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W117" s="20"/>
+      <c r="AB117" s="20"/>
       <c r="AE117" s="20"/>
       <c r="AF117" s="20"/>
     </row>
     <row r="118" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W118" s="20"/>
+      <c r="AB118" s="20"/>
       <c r="AE118" s="20"/>
       <c r="AF118" s="20"/>
     </row>
     <row r="119" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W119" s="20"/>
+      <c r="AB119" s="20"/>
       <c r="AE119" s="20"/>
       <c r="AF119" s="20"/>
     </row>
     <row r="120" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W120" s="20"/>
+      <c r="AB120" s="20"/>
       <c r="AE120" s="20"/>
       <c r="AF120" s="20"/>
     </row>
     <row r="121" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W121" s="20"/>
+      <c r="AB121" s="20"/>
       <c r="AE121" s="20"/>
       <c r="AF121" s="20"/>
     </row>
     <row r="122" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W122" s="20"/>
+      <c r="AB122" s="20"/>
       <c r="AE122" s="20"/>
       <c r="AF122" s="20"/>
     </row>
     <row r="123" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W123" s="20"/>
+      <c r="AB123" s="20"/>
       <c r="AE123" s="20"/>
       <c r="AF123" s="20"/>
     </row>
     <row r="124" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W124" s="20"/>
+      <c r="AB124" s="20"/>
       <c r="AE124" s="20"/>
       <c r="AF124" s="20"/>
     </row>
     <row r="125" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W125" s="20"/>
+      <c r="AB125" s="20"/>
       <c r="AE125" s="20"/>
       <c r="AF125" s="20"/>
     </row>
     <row r="126" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W126" s="20"/>
+      <c r="AB126" s="20"/>
       <c r="AE126" s="20"/>
       <c r="AF126" s="20"/>
     </row>
     <row r="127" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W127" s="20"/>
+      <c r="AB127" s="20"/>
       <c r="AE127" s="20"/>
       <c r="AF127" s="20"/>
     </row>
     <row r="128" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W128" s="20"/>
+      <c r="AB128" s="20"/>
       <c r="AE128" s="20"/>
       <c r="AF128" s="20"/>
     </row>
     <row r="129" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W129" s="20"/>
+      <c r="AB129" s="20"/>
       <c r="AE129" s="20"/>
       <c r="AF129" s="20"/>
     </row>
     <row r="130" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W130" s="20"/>
+      <c r="AB130" s="20"/>
       <c r="AE130" s="20"/>
       <c r="AF130" s="20"/>
     </row>
     <row r="131" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W131" s="20"/>
+      <c r="AB131" s="20"/>
       <c r="AE131" s="20"/>
       <c r="AF131" s="20"/>
     </row>
     <row r="132" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W132" s="20"/>
+      <c r="AB132" s="20"/>
       <c r="AE132" s="20"/>
       <c r="AF132" s="20"/>
     </row>
     <row r="133" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W133" s="20"/>
+      <c r="AB133" s="20"/>
       <c r="AE133" s="20"/>
       <c r="AF133" s="20"/>
     </row>
     <row r="134" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W134" s="20"/>
+      <c r="AB134" s="20"/>
       <c r="AE134" s="20"/>
       <c r="AF134" s="20"/>
     </row>
     <row r="135" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W135" s="20"/>
+      <c r="AB135" s="20"/>
       <c r="AE135" s="20"/>
       <c r="AF135" s="20"/>
     </row>
     <row r="136" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W136" s="20"/>
+      <c r="AB136" s="20"/>
       <c r="AE136" s="20"/>
       <c r="AF136" s="20"/>
     </row>
     <row r="137" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W137" s="20"/>
+      <c r="AB137" s="20"/>
       <c r="AE137" s="20"/>
       <c r="AF137" s="20"/>
     </row>
     <row r="138" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W138" s="20"/>
+      <c r="AB138" s="20"/>
       <c r="AE138" s="20"/>
       <c r="AF138" s="20"/>
     </row>
     <row r="139" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W139" s="20"/>
+      <c r="AB139" s="20"/>
       <c r="AE139" s="20"/>
       <c r="AF139" s="20"/>
     </row>
     <row r="140" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W140" s="20"/>
+      <c r="AB140" s="20"/>
       <c r="AE140" s="20"/>
       <c r="AF140" s="20"/>
     </row>
     <row r="141" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W141" s="20"/>
+      <c r="AB141" s="20"/>
       <c r="AE141" s="20"/>
       <c r="AF141" s="20"/>
     </row>
     <row r="142" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W142" s="20"/>
+      <c r="AB142" s="20"/>
       <c r="AE142" s="20"/>
       <c r="AF142" s="20"/>
     </row>
     <row r="143" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W143" s="20"/>
+      <c r="AB143" s="20"/>
       <c r="AE143" s="20"/>
       <c r="AF143" s="20"/>
     </row>
     <row r="144" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W144" s="20"/>
+      <c r="AB144" s="20"/>
       <c r="AE144" s="20"/>
       <c r="AF144" s="20"/>
     </row>
     <row r="145" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W145" s="20"/>
+      <c r="AB145" s="20"/>
       <c r="AE145" s="20"/>
       <c r="AF145" s="20"/>
     </row>
     <row r="146" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W146" s="20"/>
+      <c r="AB146" s="20"/>
       <c r="AE146" s="20"/>
       <c r="AF146" s="20"/>
     </row>
     <row r="147" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W147" s="20"/>
+      <c r="AB147" s="20"/>
       <c r="AE147" s="20"/>
       <c r="AF147" s="20"/>
     </row>
     <row r="148" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W148" s="20"/>
+      <c r="AB148" s="20"/>
       <c r="AE148" s="20"/>
       <c r="AF148" s="20"/>
     </row>
     <row r="149" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W149" s="20"/>
+      <c r="AB149" s="20"/>
       <c r="AE149" s="20"/>
       <c r="AF149" s="20"/>
     </row>
     <row r="150" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W150" s="20"/>
+      <c r="AB150" s="20"/>
       <c r="AE150" s="20"/>
       <c r="AF150" s="20"/>
     </row>
     <row r="151" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W151" s="20"/>
+      <c r="AB151" s="20"/>
       <c r="AE151" s="20"/>
       <c r="AF151" s="20"/>
     </row>
     <row r="152" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W152" s="20"/>
+      <c r="AB152" s="20"/>
       <c r="AE152" s="20"/>
       <c r="AF152" s="20"/>
     </row>
     <row r="153" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W153" s="20"/>
+      <c r="AB153" s="20"/>
       <c r="AE153" s="20"/>
       <c r="AF153" s="20"/>
     </row>
     <row r="154" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W154" s="20"/>
+      <c r="AB154" s="20"/>
       <c r="AE154" s="20"/>
       <c r="AF154" s="20"/>
     </row>
     <row r="155" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W155" s="20"/>
+      <c r="AB155" s="20"/>
       <c r="AE155" s="20"/>
       <c r="AF155" s="20"/>
     </row>
     <row r="156" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W156" s="20"/>
+      <c r="AB156" s="20"/>
       <c r="AE156" s="20"/>
       <c r="AF156" s="20"/>
     </row>
     <row r="157" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W157" s="20"/>
+      <c r="AB157" s="20"/>
       <c r="AE157" s="20"/>
       <c r="AF157" s="20"/>
     </row>
     <row r="158" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W158" s="20"/>
+      <c r="AB158" s="20"/>
       <c r="AE158" s="20"/>
       <c r="AF158" s="20"/>
     </row>
     <row r="159" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W159" s="20"/>
+      <c r="AB159" s="20"/>
       <c r="AE159" s="20"/>
       <c r="AF159" s="20"/>
     </row>
     <row r="160" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W160" s="20"/>
+      <c r="AB160" s="20"/>
       <c r="AE160" s="20"/>
       <c r="AF160" s="20"/>
     </row>
     <row r="161" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W161" s="20"/>
+      <c r="AB161" s="20"/>
       <c r="AE161" s="20"/>
       <c r="AF161" s="20"/>
     </row>
     <row r="162" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W162" s="20"/>
+      <c r="AB162" s="20"/>
       <c r="AE162" s="20"/>
       <c r="AF162" s="20"/>
     </row>
     <row r="163" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W163" s="20"/>
+      <c r="AB163" s="20"/>
       <c r="AE163" s="20"/>
       <c r="AF163" s="20"/>
     </row>
     <row r="164" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W164" s="20"/>
+      <c r="AB164" s="20"/>
       <c r="AE164" s="20"/>
       <c r="AF164" s="20"/>
     </row>
     <row r="165" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W165" s="20"/>
+      <c r="AB165" s="20"/>
       <c r="AE165" s="20"/>
       <c r="AF165" s="20"/>
     </row>
     <row r="166" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W166" s="20"/>
+      <c r="AB166" s="20"/>
       <c r="AE166" s="20"/>
       <c r="AF166" s="20"/>
     </row>
     <row r="167" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W167" s="20"/>
+      <c r="AB167" s="20"/>
       <c r="AE167" s="20"/>
       <c r="AF167" s="20"/>
     </row>
     <row r="168" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W168" s="20"/>
+      <c r="AB168" s="20"/>
       <c r="AE168" s="20"/>
       <c r="AF168" s="20"/>
     </row>
     <row r="169" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W169" s="20"/>
+      <c r="AB169" s="20"/>
       <c r="AE169" s="20"/>
       <c r="AF169" s="20"/>
     </row>
     <row r="170" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W170" s="20"/>
+      <c r="AB170" s="20"/>
       <c r="AE170" s="20"/>
       <c r="AF170" s="20"/>
     </row>
     <row r="171" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W171" s="20"/>
+      <c r="AB171" s="20"/>
       <c r="AE171" s="20"/>
       <c r="AF171" s="20"/>
     </row>
     <row r="172" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W172" s="20"/>
+      <c r="AB172" s="20"/>
       <c r="AE172" s="20"/>
       <c r="AF172" s="20"/>
     </row>
     <row r="173" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W173" s="20"/>
+      <c r="AB173" s="20"/>
       <c r="AE173" s="20"/>
       <c r="AF173" s="20"/>
     </row>
     <row r="174" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W174" s="20"/>
+      <c r="AB174" s="20"/>
       <c r="AE174" s="20"/>
       <c r="AF174" s="20"/>
     </row>
     <row r="175" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W175" s="20"/>
+      <c r="AB175" s="20"/>
       <c r="AE175" s="20"/>
       <c r="AF175" s="20"/>
     </row>
     <row r="176" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W176" s="20"/>
+      <c r="AB176" s="20"/>
       <c r="AE176" s="20"/>
       <c r="AF176" s="20"/>
     </row>
     <row r="177" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W177" s="20"/>
+      <c r="AB177" s="20"/>
       <c r="AE177" s="20"/>
       <c r="AF177" s="20"/>
     </row>
     <row r="178" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W178" s="20"/>
+      <c r="AB178" s="20"/>
       <c r="AE178" s="20"/>
       <c r="AF178" s="20"/>
     </row>
     <row r="179" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W179" s="20"/>
+      <c r="AB179" s="20"/>
       <c r="AE179" s="20"/>
       <c r="AF179" s="20"/>
     </row>
     <row r="180" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W180" s="20"/>
+      <c r="AB180" s="20"/>
       <c r="AE180" s="20"/>
       <c r="AF180" s="20"/>
     </row>
     <row r="181" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W181" s="20"/>
+      <c r="AB181" s="20"/>
       <c r="AE181" s="20"/>
       <c r="AF181" s="20"/>
     </row>
     <row r="182" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W182" s="20"/>
+      <c r="AB182" s="20"/>
       <c r="AE182" s="20"/>
       <c r="AF182" s="20"/>
     </row>
     <row r="183" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W183" s="20"/>
+      <c r="AB183" s="20"/>
       <c r="AE183" s="20"/>
       <c r="AF183" s="20"/>
     </row>
     <row r="184" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W184" s="20"/>
+      <c r="AB184" s="20"/>
       <c r="AE184" s="20"/>
       <c r="AF184" s="20"/>
     </row>
     <row r="185" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W185" s="20"/>
+      <c r="AB185" s="20"/>
       <c r="AE185" s="20"/>
       <c r="AF185" s="20"/>
     </row>
     <row r="186" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W186" s="20"/>
+      <c r="AB186" s="20"/>
       <c r="AE186" s="20"/>
       <c r="AF186" s="20"/>
     </row>
     <row r="187" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W187" s="20"/>
+      <c r="AB187" s="20"/>
       <c r="AE187" s="20"/>
       <c r="AF187" s="20"/>
     </row>
     <row r="188" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W188" s="20"/>
+      <c r="AB188" s="20"/>
       <c r="AE188" s="20"/>
       <c r="AF188" s="20"/>
     </row>
     <row r="189" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W189" s="20"/>
+      <c r="AB189" s="20"/>
       <c r="AE189" s="20"/>
       <c r="AF189" s="20"/>
     </row>
     <row r="190" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W190" s="20"/>
+      <c r="AB190" s="20"/>
       <c r="AE190" s="20"/>
       <c r="AF190" s="20"/>
     </row>
     <row r="191" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W191" s="20"/>
+      <c r="AB191" s="20"/>
       <c r="AE191" s="20"/>
       <c r="AF191" s="20"/>
     </row>
     <row r="192" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W192" s="20"/>
+      <c r="AB192" s="20"/>
       <c r="AE192" s="20"/>
       <c r="AF192" s="20"/>
     </row>
     <row r="193" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W193" s="20"/>
+      <c r="AB193" s="20"/>
       <c r="AE193" s="20"/>
       <c r="AF193" s="20"/>
     </row>
     <row r="194" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W194" s="20"/>
+      <c r="AB194" s="20"/>
       <c r="AE194" s="20"/>
       <c r="AF194" s="20"/>
     </row>
     <row r="195" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W195" s="20"/>
+      <c r="AB195" s="20"/>
       <c r="AE195" s="20"/>
       <c r="AF195" s="20"/>
     </row>
     <row r="196" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W196" s="20"/>
+      <c r="AB196" s="20"/>
       <c r="AE196" s="20"/>
       <c r="AF196" s="20"/>
     </row>
     <row r="197" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W197" s="20"/>
+      <c r="AB197" s="20"/>
       <c r="AE197" s="20"/>
       <c r="AF197" s="20"/>
     </row>
     <row r="198" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W198" s="20"/>
+      <c r="AB198" s="20"/>
       <c r="AE198" s="20"/>
       <c r="AF198" s="20"/>
     </row>
     <row r="199" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="W199" s="20"/>
+      <c r="AB199" s="20"/>
       <c r="AE199" s="20"/>
       <c r="AF199" s="20"/>
     </row>
     <row r="200" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB200" s="20"/>
       <c r="AE200" s="20"/>
       <c r="AF200" s="20"/>
+    </row>
+    <row r="201" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB201" s="20"/>
+    </row>
+    <row r="202" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB202" s="20"/>
+    </row>
+    <row r="203" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB203" s="20"/>
+    </row>
+    <row r="204" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB204" s="20"/>
+    </row>
+    <row r="205" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB205" s="20"/>
+    </row>
+    <row r="206" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB206" s="20"/>
+    </row>
+    <row r="207" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB207" s="20"/>
+    </row>
+    <row r="208" spans="23:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB208" s="20"/>
+    </row>
+    <row r="209" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB209" s="20"/>
+    </row>
+    <row r="210" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB210" s="20"/>
+    </row>
+    <row r="211" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB211" s="20"/>
+    </row>
+    <row r="212" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB212" s="20"/>
+    </row>
+    <row r="213" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB213" s="20"/>
+    </row>
+    <row r="214" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB214" s="20"/>
+    </row>
+    <row r="215" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB215" s="20"/>
+    </row>
+    <row r="216" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB216" s="20"/>
+    </row>
+    <row r="217" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB217" s="20"/>
+    </row>
+    <row r="218" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB218" s="20"/>
+    </row>
+    <row r="219" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB219" s="20"/>
+    </row>
+    <row r="220" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB220" s="20"/>
+    </row>
+    <row r="221" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB221" s="20"/>
+    </row>
+    <row r="222" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB222" s="20"/>
+    </row>
+    <row r="223" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB223" s="20"/>
+    </row>
+    <row r="224" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB224" s="20"/>
+    </row>
+    <row r="225" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB225" s="20"/>
+    </row>
+    <row r="226" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB226" s="20"/>
+    </row>
+    <row r="227" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB227" s="20"/>
+    </row>
+    <row r="228" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB228" s="20"/>
+    </row>
+    <row r="229" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB229" s="20"/>
+    </row>
+    <row r="230" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB230" s="20"/>
+    </row>
+    <row r="231" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB231" s="20"/>
+    </row>
+    <row r="232" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB232" s="20"/>
+    </row>
+    <row r="233" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB233" s="20"/>
+    </row>
+    <row r="234" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB234" s="20"/>
+    </row>
+    <row r="235" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB235" s="20"/>
+    </row>
+    <row r="236" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB236" s="20"/>
+    </row>
+    <row r="237" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB237" s="20"/>
+    </row>
+    <row r="238" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB238" s="20"/>
+    </row>
+    <row r="239" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB239" s="20"/>
+    </row>
+    <row r="240" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB240" s="20"/>
+    </row>
+    <row r="241" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB241" s="20"/>
+    </row>
+    <row r="242" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB242" s="20"/>
+    </row>
+    <row r="243" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB243" s="20"/>
+    </row>
+    <row r="244" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB244" s="20"/>
+    </row>
+    <row r="245" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB245" s="20"/>
+    </row>
+    <row r="246" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB246" s="20"/>
+    </row>
+    <row r="247" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB247" s="20"/>
+    </row>
+    <row r="248" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB248" s="20"/>
+    </row>
+    <row r="249" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB249" s="20"/>
+    </row>
+    <row r="250" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB250" s="20"/>
+    </row>
+    <row r="251" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB251" s="20"/>
+    </row>
+    <row r="252" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB252" s="20"/>
+    </row>
+    <row r="253" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB253" s="20"/>
+    </row>
+    <row r="254" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB254" s="20"/>
+    </row>
+    <row r="255" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB255" s="20"/>
+    </row>
+    <row r="256" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB256" s="20"/>
+    </row>
+    <row r="257" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB257" s="20"/>
+    </row>
+    <row r="258" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB258" s="20"/>
+    </row>
+    <row r="259" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB259" s="20"/>
+    </row>
+    <row r="260" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB260" s="20"/>
+    </row>
+    <row r="261" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB261" s="20"/>
+    </row>
+    <row r="262" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB262" s="20"/>
+    </row>
+    <row r="263" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB263" s="20"/>
+    </row>
+    <row r="264" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB264" s="20"/>
+    </row>
+    <row r="265" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB265" s="20"/>
+    </row>
+    <row r="266" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB266" s="20"/>
+    </row>
+    <row r="267" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB267" s="20"/>
+    </row>
+    <row r="268" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB268" s="20"/>
+    </row>
+    <row r="269" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB269" s="20"/>
+    </row>
+    <row r="270" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB270" s="20"/>
+    </row>
+    <row r="271" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB271" s="20"/>
+    </row>
+    <row r="272" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB272" s="20"/>
+    </row>
+    <row r="273" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB273" s="20"/>
+    </row>
+    <row r="274" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB274" s="20"/>
+    </row>
+    <row r="275" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB275" s="20"/>
+    </row>
+    <row r="276" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB276" s="20"/>
+    </row>
+    <row r="277" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB277" s="20"/>
+    </row>
+    <row r="278" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB278" s="20"/>
+    </row>
+    <row r="279" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB279" s="20"/>
+    </row>
+    <row r="280" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB280" s="20"/>
+    </row>
+    <row r="281" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB281" s="20"/>
+    </row>
+    <row r="282" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB282" s="20"/>
+    </row>
+    <row r="283" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB283" s="20"/>
+    </row>
+    <row r="284" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB284" s="20"/>
+    </row>
+    <row r="285" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB285" s="20"/>
+    </row>
+    <row r="286" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB286" s="20"/>
+    </row>
+    <row r="287" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB287" s="20"/>
+    </row>
+    <row r="288" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB288" s="20"/>
+    </row>
+    <row r="289" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB289" s="20"/>
+    </row>
+    <row r="290" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB290" s="20"/>
+    </row>
+    <row r="291" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB291" s="20"/>
+    </row>
+    <row r="292" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB292" s="20"/>
+    </row>
+    <row r="293" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB293" s="20"/>
+    </row>
+    <row r="294" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB294" s="20"/>
+    </row>
+    <row r="295" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB295" s="20"/>
+    </row>
+    <row r="296" spans="28:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB296" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -7675,19 +8133,19 @@
         <v>2017</v>
       </c>
       <c r="C23" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>605</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>606</v>
-      </c>
       <c r="E23" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="F23" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>583</v>
-      </c>
       <c r="G23" s="22" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -7698,7 +8156,7 @@
         <v>516</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E24" s="23">
         <v>2</v>
@@ -7718,7 +8176,7 @@
         <v>516</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E25" s="23">
         <v>2</v>
@@ -7735,10 +8193,10 @@
         <v>2021</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E26" s="23">
         <v>4</v>
@@ -7755,10 +8213,10 @@
         <v>2007</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E27" s="23">
         <v>2</v>
@@ -7775,10 +8233,10 @@
         <v>2023</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E28" s="23">
         <v>1</v>
@@ -7795,10 +8253,10 @@
         <v>2022</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E29" s="23">
         <v>5</v>
@@ -7815,10 +8273,10 @@
         <v>2022</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E30" s="23" t="s">
         <v>40</v>
@@ -7838,7 +8296,7 @@
         <v>514</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E31" s="23">
         <v>7</v>
@@ -7855,7 +8313,7 @@
         <v>514</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E32" s="23">
         <v>1</v>
@@ -7872,7 +8330,7 @@
         <v>514</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E33" s="23">
         <v>3</v>
@@ -7889,7 +8347,7 @@
         <v>514</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E34" s="23">
         <v>2</v>
@@ -7906,7 +8364,7 @@
         <v>514</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E35" s="23">
         <v>4</v>
@@ -7923,7 +8381,7 @@
         <v>514</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E36" s="23">
         <v>3</v>
@@ -7940,7 +8398,7 @@
         <v>517</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E37" s="23">
         <v>1</v>
@@ -7957,7 +8415,7 @@
         <v>518</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E38" s="23">
         <v>2</v>
@@ -7974,7 +8432,7 @@
         <v>518</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E39" s="23">
         <v>1</v>

</xml_diff>

<commit_message>
update after impact and outcome analysis
</commit_message>
<xml_diff>
--- a/Data Extraction Sheet.xlsx
+++ b/Data Extraction Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/rw3031_cumc_columbia_edu/Documents/Documents/EveryBreathMatters/systematic review/lungcancer_tech_slr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1E4814F-8BE4-4E24-BAB3-7DCD0B8CAB39}"/>
+  <xr:revisionPtr revIDLastSave="394" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{943190FA-194C-40D6-B447-71A5283CDC6C}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="636">
   <si>
     <t>Title</t>
   </si>
@@ -1904,18 +1904,9 @@
     <t>communication and coordination,education and information delivery</t>
   </si>
   <si>
-    <t>education and information delivery,decision support and guidance</t>
-  </si>
-  <si>
     <t>communication and coordination,emotional and social support</t>
   </si>
   <si>
-    <t>monitoring and tracking,communication and coordination,education and information delivery,decision support and guidance</t>
-  </si>
-  <si>
-    <t>education and information delivery,emotional and social support,promotion of healthy behavior</t>
-  </si>
-  <si>
     <t>communication and coordination</t>
   </si>
   <si>
@@ -1925,18 +1916,12 @@
     <t>mobile application</t>
   </si>
   <si>
-    <t>During-treatment,Post-treatment</t>
-  </si>
-  <si>
     <t>During-treatment</t>
   </si>
   <si>
     <t>Post-treatment</t>
   </si>
   <si>
-    <t>Pre-treatment,During-treatment,Post-treatment</t>
-  </si>
-  <si>
     <t>Pre-treatment</t>
   </si>
   <si>
@@ -2147,13 +2132,16 @@
     <t>education and information delivery</t>
   </si>
   <si>
-    <t>monitoring and tracking,decision support and guidance</t>
-  </si>
-  <si>
     <t>monitoring and tracking,promotion of healthy behavior</t>
   </si>
   <si>
-    <t>monitoring and tracking,decision support and guidance,emotional and social support</t>
+    <t>monitoring and tracking,education and information delivery</t>
+  </si>
+  <si>
+    <t>monitoring and tracking,communication and coordination,education and information delivery</t>
+  </si>
+  <si>
+    <t>Pre-treatment, Post-treatment</t>
   </si>
 </sst>
 </file>
@@ -2306,7 +2294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2327,12 +2315,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2708,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y11" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AF28" sqref="AF28"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2735,7 +2717,7 @@
     <col min="20" max="20" width="18.6328125" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="45.453125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="16.81640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="41.54296875" style="13" customWidth="1"/>
+    <col min="23" max="23" width="41.54296875" style="11" customWidth="1"/>
     <col min="24" max="24" width="55.1796875" customWidth="1"/>
     <col min="25" max="26" width="38.36328125" customWidth="1"/>
     <col min="27" max="27" width="34.54296875" customWidth="1"/>
@@ -2813,8 +2795,8 @@
       <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="11" t="s">
-        <v>561</v>
+      <c r="W1" s="10" t="s">
+        <v>558</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>21</v>
@@ -2823,7 +2805,7 @@
         <v>22</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>23</v>
@@ -2832,7 +2814,7 @@
         <v>24</v>
       </c>
       <c r="AC1" s="10" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>533</v>
@@ -2841,16 +2823,16 @@
         <v>548</v>
       </c>
       <c r="AF1" s="10" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="AG1" s="10" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2917,8 +2899,8 @@
       <c r="V2" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="12" t="s">
-        <v>550</v>
+      <c r="W2" s="9" t="s">
+        <v>581</v>
       </c>
       <c r="X2" t="s">
         <v>41</v>
@@ -2927,7 +2909,7 @@
         <v>42</v>
       </c>
       <c r="Z2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="AA2" t="s">
         <v>43</v>
@@ -2945,13 +2927,13 @@
         <v>539</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="AH2" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3021,7 +3003,7 @@
       <c r="V3" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="9" t="s">
         <v>552</v>
       </c>
       <c r="X3" t="s">
@@ -3031,7 +3013,7 @@
         <v>59</v>
       </c>
       <c r="Z3" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="AA3" t="s">
         <v>60</v>
@@ -3040,7 +3022,7 @@
         <v>61</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD3">
         <v>1.5</v>
@@ -3049,16 +3031,16 @@
         <v>55</v>
       </c>
       <c r="AF3" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG3" s="9" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="AH3" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3125,7 +3107,7 @@
       <c r="V4" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="9" t="s">
         <v>550</v>
       </c>
       <c r="X4" t="s">
@@ -3144,7 +3126,7 @@
         <v>76</v>
       </c>
       <c r="AC4" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD4">
         <v>3</v>
@@ -3153,13 +3135,13 @@
         <v>55</v>
       </c>
       <c r="AF4" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG4" s="9" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="AH4" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3229,8 +3211,8 @@
       <c r="V5" t="s">
         <v>40</v>
       </c>
-      <c r="W5" s="12" t="s">
-        <v>638</v>
+      <c r="W5" s="9" t="s">
+        <v>632</v>
       </c>
       <c r="X5" t="s">
         <v>91</v>
@@ -3239,7 +3221,7 @@
         <v>98</v>
       </c>
       <c r="Z5" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="AA5" t="s">
         <v>99</v>
@@ -3248,7 +3230,7 @@
         <v>92</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -3257,16 +3239,16 @@
         <v>540</v>
       </c>
       <c r="AF5" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="AG5" s="9" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="AH5" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3333,8 +3315,8 @@
       <c r="V6" t="s">
         <v>40</v>
       </c>
-      <c r="W6" s="12" t="s">
-        <v>635</v>
+      <c r="W6" s="9" t="s">
+        <v>630</v>
       </c>
       <c r="X6" t="s">
         <v>116</v>
@@ -3343,7 +3325,7 @@
         <v>118</v>
       </c>
       <c r="Z6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="AA6" t="s">
         <v>129</v>
@@ -3361,16 +3343,16 @@
         <v>541</v>
       </c>
       <c r="AF6" s="9" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="AG6" s="9" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="AH6" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3437,8 +3419,8 @@
       <c r="V7" t="s">
         <v>40</v>
       </c>
-      <c r="W7" s="12" t="s">
-        <v>553</v>
+      <c r="W7" s="9" t="s">
+        <v>556</v>
       </c>
       <c r="X7" t="s">
         <v>139</v>
@@ -3447,7 +3429,7 @@
         <v>140</v>
       </c>
       <c r="Z7" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="AA7" t="s">
         <v>141</v>
@@ -3465,16 +3447,16 @@
         <v>542</v>
       </c>
       <c r="AF7" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG7" s="9" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="AH7" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3541,8 +3523,8 @@
       <c r="V8" t="s">
         <v>40</v>
       </c>
-      <c r="W8" s="12" t="s">
-        <v>551</v>
+      <c r="W8" s="9" t="s">
+        <v>557</v>
       </c>
       <c r="X8" t="s">
         <v>117</v>
@@ -3551,7 +3533,7 @@
         <v>148</v>
       </c>
       <c r="Z8" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="AA8" t="s">
         <v>119</v>
@@ -3569,13 +3551,13 @@
         <v>543</v>
       </c>
       <c r="AF8" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG8" s="9" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="AH8" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3645,8 +3627,8 @@
       <c r="V9" t="s">
         <v>177</v>
       </c>
-      <c r="W9" s="12" t="s">
-        <v>586</v>
+      <c r="W9" s="9" t="s">
+        <v>581</v>
       </c>
       <c r="X9" t="s">
         <v>178</v>
@@ -3655,7 +3637,7 @@
         <v>167</v>
       </c>
       <c r="Z9" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="AA9" t="s">
         <v>179</v>
@@ -3673,16 +3655,16 @@
         <v>540</v>
       </c>
       <c r="AF9" s="9" t="s">
-        <v>566</v>
+        <v>635</v>
       </c>
       <c r="AG9" s="9" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="AH9" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3749,8 +3731,8 @@
       <c r="V10" t="s">
         <v>40</v>
       </c>
-      <c r="W10" s="12" t="s">
-        <v>639</v>
+      <c r="W10" s="9" t="s">
+        <v>553</v>
       </c>
       <c r="X10" t="s">
         <v>161</v>
@@ -3759,7 +3741,7 @@
         <v>160</v>
       </c>
       <c r="Z10" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="AA10" t="s">
         <v>159</v>
@@ -3777,13 +3759,13 @@
         <v>539</v>
       </c>
       <c r="AF10" s="9" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="AG10" s="9" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="AH10" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3853,7 +3835,7 @@
       <c r="V11" t="s">
         <v>188</v>
       </c>
-      <c r="W11" s="12" t="s">
+      <c r="W11" s="9" t="s">
         <v>554</v>
       </c>
       <c r="X11" t="s">
@@ -3881,16 +3863,16 @@
         <v>55</v>
       </c>
       <c r="AF11" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG11" s="9" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="AH11" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3957,9 +3939,7 @@
       <c r="V12" t="s">
         <v>210</v>
       </c>
-      <c r="W12" s="12" t="s">
-        <v>555</v>
-      </c>
+      <c r="W12" s="9"/>
       <c r="X12" t="s">
         <v>204</v>
       </c>
@@ -3967,7 +3947,7 @@
         <v>213</v>
       </c>
       <c r="Z12" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="AA12" t="s">
         <v>212</v>
@@ -3985,16 +3965,16 @@
         <v>544</v>
       </c>
       <c r="AF12" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG12" s="9" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="AH12" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4061,8 +4041,8 @@
       <c r="V13" t="s">
         <v>40</v>
       </c>
-      <c r="W13" s="12" t="s">
-        <v>551</v>
+      <c r="W13" s="9" t="s">
+        <v>557</v>
       </c>
       <c r="X13" t="s">
         <v>228</v>
@@ -4071,7 +4051,7 @@
         <v>223</v>
       </c>
       <c r="Z13" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="AA13" t="s">
         <v>229</v>
@@ -4089,16 +4069,16 @@
         <v>55</v>
       </c>
       <c r="AF13" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG13" s="9" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="AH13" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4165,8 +4145,8 @@
       <c r="V14" t="s">
         <v>241</v>
       </c>
-      <c r="W14" s="12" t="s">
-        <v>551</v>
+      <c r="W14" s="9" t="s">
+        <v>555</v>
       </c>
       <c r="X14" t="s">
         <v>242</v>
@@ -4175,7 +4155,7 @@
         <v>244</v>
       </c>
       <c r="Z14" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="AA14" t="s">
         <v>243</v>
@@ -4193,16 +4173,16 @@
         <v>544</v>
       </c>
       <c r="AF14" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG14" s="9" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="AH14" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4269,7 +4249,7 @@
       <c r="V15" t="s">
         <v>40</v>
       </c>
-      <c r="W15" s="12" t="s">
+      <c r="W15" s="9" t="s">
         <v>551</v>
       </c>
       <c r="X15" t="s">
@@ -4279,7 +4259,7 @@
         <v>259</v>
       </c>
       <c r="Z15" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="AA15" t="s">
         <v>258</v>
@@ -4288,7 +4268,7 @@
         <v>260</v>
       </c>
       <c r="AC15" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD15">
         <v>18</v>
@@ -4297,16 +4277,16 @@
         <v>539</v>
       </c>
       <c r="AF15" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="AG15" s="9" t="s">
         <v>565</v>
       </c>
-      <c r="AG15" s="9" t="s">
-        <v>570</v>
-      </c>
       <c r="AH15" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4373,7 +4353,7 @@
       <c r="V16" t="s">
         <v>40</v>
       </c>
-      <c r="W16" s="12" t="s">
+      <c r="W16" s="9" t="s">
         <v>551</v>
       </c>
       <c r="X16" t="s">
@@ -4383,7 +4363,7 @@
         <v>273</v>
       </c>
       <c r="Z16" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="AA16" t="s">
         <v>274</v>
@@ -4392,7 +4372,7 @@
         <v>269</v>
       </c>
       <c r="AC16" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD16">
         <v>15</v>
@@ -4401,16 +4381,16 @@
         <v>55</v>
       </c>
       <c r="AF16" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG16" s="9" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="AH16" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4477,8 +4457,8 @@
       <c r="V17" t="s">
         <v>40</v>
       </c>
-      <c r="W17" s="12" t="s">
-        <v>556</v>
+      <c r="W17" s="9" t="s">
+        <v>631</v>
       </c>
       <c r="X17" t="s">
         <v>288</v>
@@ -4487,7 +4467,7 @@
         <v>290</v>
       </c>
       <c r="Z17" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="AA17" t="s">
         <v>289</v>
@@ -4505,16 +4485,16 @@
         <v>544</v>
       </c>
       <c r="AF17" s="9" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="AG17" s="9" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="AH17" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4581,8 +4561,8 @@
       <c r="V18" t="s">
         <v>40</v>
       </c>
-      <c r="W18" s="12" t="s">
-        <v>557</v>
+      <c r="W18" s="9" t="s">
+        <v>556</v>
       </c>
       <c r="X18" t="s">
         <v>299</v>
@@ -4591,7 +4571,7 @@
         <v>304</v>
       </c>
       <c r="Z18" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="AA18" t="s">
         <v>305</v>
@@ -4609,13 +4589,13 @@
         <v>540</v>
       </c>
       <c r="AF18" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="AG18" s="9" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="AH18" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4685,8 +4665,8 @@
       <c r="V19" t="s">
         <v>281</v>
       </c>
-      <c r="W19" s="12" t="s">
-        <v>636</v>
+      <c r="W19" s="9" t="s">
+        <v>633</v>
       </c>
       <c r="X19" t="s">
         <v>312</v>
@@ -4695,7 +4675,7 @@
         <v>313</v>
       </c>
       <c r="Z19" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="AA19" t="s">
         <v>314</v>
@@ -4713,13 +4693,13 @@
         <v>544</v>
       </c>
       <c r="AF19" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG19" s="9" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="AH19" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4789,8 +4769,8 @@
       <c r="V20" t="s">
         <v>182</v>
       </c>
-      <c r="W20" s="12" t="s">
-        <v>636</v>
+      <c r="W20" s="9" t="s">
+        <v>581</v>
       </c>
       <c r="X20" t="s">
         <v>348</v>
@@ -4799,7 +4779,7 @@
         <v>347</v>
       </c>
       <c r="Z20" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="AA20" t="s">
         <v>344</v>
@@ -4817,13 +4797,13 @@
         <v>544</v>
       </c>
       <c r="AF20" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG20" s="9" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="AH20" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4893,9 +4873,7 @@
       <c r="V21" t="s">
         <v>323</v>
       </c>
-      <c r="W21" s="12" t="s">
-        <v>552</v>
-      </c>
+      <c r="W21" s="9"/>
       <c r="X21" t="s">
         <v>335</v>
       </c>
@@ -4903,7 +4881,7 @@
         <v>334</v>
       </c>
       <c r="Z21" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="AA21" t="s">
         <v>324</v>
@@ -4921,16 +4899,16 @@
         <v>544</v>
       </c>
       <c r="AF21" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG21" s="9" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="AH21" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4997,7 +4975,7 @@
       <c r="V22" t="s">
         <v>40</v>
       </c>
-      <c r="W22" s="12" t="s">
+      <c r="W22" s="9" t="s">
         <v>551</v>
       </c>
       <c r="X22" t="s">
@@ -5007,13 +4985,13 @@
         <v>352</v>
       </c>
       <c r="Z22" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="AA22" t="s">
         <v>360</v>
       </c>
       <c r="AC22" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD22">
         <v>13</v>
@@ -5022,13 +5000,13 @@
         <v>545</v>
       </c>
       <c r="AF22" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="AG22" s="9" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="AH22" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5086,12 +5064,12 @@
       <c r="V23" t="s">
         <v>40</v>
       </c>
-      <c r="W23" s="12"/>
+      <c r="W23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AF23" s="9"/>
       <c r="AG23" s="9"/>
     </row>
-    <row r="24" spans="1:34" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5158,8 +5136,8 @@
       <c r="V24" t="s">
         <v>40</v>
       </c>
-      <c r="W24" s="12" t="s">
-        <v>558</v>
+      <c r="W24" s="9" t="s">
+        <v>634</v>
       </c>
       <c r="X24" t="s">
         <v>363</v>
@@ -5168,7 +5146,7 @@
         <v>372</v>
       </c>
       <c r="Z24" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="AA24" t="s">
         <v>373</v>
@@ -5177,7 +5155,7 @@
         <v>374</v>
       </c>
       <c r="AC24" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD24">
         <v>6</v>
@@ -5186,16 +5164,16 @@
         <v>55</v>
       </c>
       <c r="AF24" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG24" s="9" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="AH24" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5262,8 +5240,8 @@
       <c r="V25" t="s">
         <v>40</v>
       </c>
-      <c r="W25" s="12" t="s">
-        <v>559</v>
+      <c r="W25" s="9" t="s">
+        <v>550</v>
       </c>
       <c r="X25" t="s">
         <v>396</v>
@@ -5272,7 +5250,7 @@
         <v>391</v>
       </c>
       <c r="Z25" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="AA25" t="s">
         <v>397</v>
@@ -5290,13 +5268,13 @@
         <v>539</v>
       </c>
       <c r="AF25" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="AG25" s="9" t="s">
         <v>564</v>
       </c>
-      <c r="AG25" s="9" t="s">
-        <v>569</v>
-      </c>
       <c r="AH25" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5366,8 +5344,8 @@
       <c r="V26" t="s">
         <v>182</v>
       </c>
-      <c r="W26" s="12" t="s">
-        <v>560</v>
+      <c r="W26" s="9" t="s">
+        <v>557</v>
       </c>
       <c r="X26" t="s">
         <v>409</v>
@@ -5376,7 +5354,7 @@
         <v>412</v>
       </c>
       <c r="Z26" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="AA26" t="s">
         <v>411</v>
@@ -5394,13 +5372,13 @@
         <v>546</v>
       </c>
       <c r="AF26" s="9" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="AG26" s="9" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="AH26" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5470,8 +5448,8 @@
       <c r="V27" t="s">
         <v>182</v>
       </c>
-      <c r="W27" s="12" t="s">
-        <v>560</v>
+      <c r="W27" s="9" t="s">
+        <v>557</v>
       </c>
       <c r="X27" t="s">
         <v>428</v>
@@ -5480,7 +5458,7 @@
         <v>429</v>
       </c>
       <c r="Z27" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="AA27" t="s">
         <v>430</v>
@@ -5498,16 +5476,16 @@
         <v>55</v>
       </c>
       <c r="AF27" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG27" s="9" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="AH27" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5574,8 +5552,8 @@
       <c r="V28" t="s">
         <v>182</v>
       </c>
-      <c r="W28" s="12" t="s">
-        <v>637</v>
+      <c r="W28" s="9" t="s">
+        <v>551</v>
       </c>
       <c r="X28" t="s">
         <v>444</v>
@@ -5593,22 +5571,22 @@
         <v>446</v>
       </c>
       <c r="AC28" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AD28">
         <v>0</v>
       </c>
       <c r="AE28" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="AF28" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG28" s="9" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="AH28" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5678,9 +5656,7 @@
       <c r="V29" t="s">
         <v>457</v>
       </c>
-      <c r="W29" s="12" t="s">
-        <v>552</v>
-      </c>
+      <c r="W29" s="9"/>
       <c r="X29" t="s">
         <v>461</v>
       </c>
@@ -5688,7 +5664,7 @@
         <v>463</v>
       </c>
       <c r="Z29" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="AA29" t="s">
         <v>462</v>
@@ -5700,16 +5676,16 @@
         <v>508</v>
       </c>
       <c r="AE29" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="AF29" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG29" s="9" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="AH29" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="30" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5779,8 +5755,8 @@
       <c r="V30" t="s">
         <v>182</v>
       </c>
-      <c r="W30" s="12" t="s">
-        <v>586</v>
+      <c r="W30" s="9" t="s">
+        <v>581</v>
       </c>
       <c r="X30" t="s">
         <v>476</v>
@@ -5789,7 +5765,7 @@
         <v>478</v>
       </c>
       <c r="Z30" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="AA30" t="s">
         <v>475</v>
@@ -5804,1025 +5780,1025 @@
         <v>547</v>
       </c>
       <c r="AF30" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="AG30" s="9" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="AH30" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
     </row>
     <row r="31" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W31" s="12"/>
+      <c r="W31" s="9"/>
       <c r="AC31" s="9"/>
       <c r="AF31" s="9"/>
       <c r="AG31" s="9"/>
     </row>
     <row r="32" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W32" s="12"/>
+      <c r="W32" s="9"/>
       <c r="AC32" s="9"/>
       <c r="AF32" s="9"/>
       <c r="AG32" s="9"/>
     </row>
     <row r="33" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W33" s="12"/>
+      <c r="W33" s="9"/>
       <c r="AC33" s="9"/>
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
     </row>
     <row r="34" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W34" s="12"/>
+      <c r="W34" s="9"/>
       <c r="AC34" s="9"/>
       <c r="AF34" s="9"/>
       <c r="AG34" s="9"/>
     </row>
     <row r="35" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W35" s="12"/>
+      <c r="W35" s="9"/>
       <c r="AC35" s="9"/>
       <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
     </row>
     <row r="36" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W36" s="12"/>
+      <c r="W36" s="9"/>
       <c r="AC36" s="9"/>
       <c r="AF36" s="9"/>
       <c r="AG36" s="9"/>
     </row>
     <row r="37" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W37" s="12"/>
+      <c r="W37" s="9"/>
       <c r="AC37" s="9"/>
       <c r="AF37" s="9"/>
       <c r="AG37" s="9"/>
     </row>
     <row r="38" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W38" s="12"/>
+      <c r="W38" s="9"/>
       <c r="AC38" s="9"/>
       <c r="AF38" s="9"/>
       <c r="AG38" s="9"/>
     </row>
     <row r="39" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W39" s="12"/>
+      <c r="W39" s="9"/>
       <c r="AC39" s="9"/>
       <c r="AF39" s="9"/>
       <c r="AG39" s="9"/>
     </row>
     <row r="40" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W40" s="12"/>
+      <c r="W40" s="9"/>
       <c r="AC40" s="9"/>
       <c r="AF40" s="9"/>
       <c r="AG40" s="9"/>
     </row>
     <row r="41" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W41" s="12"/>
+      <c r="W41" s="9"/>
       <c r="AC41" s="9"/>
       <c r="AF41" s="9"/>
       <c r="AG41" s="9"/>
     </row>
     <row r="42" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W42" s="12"/>
+      <c r="W42" s="9"/>
       <c r="AC42" s="9"/>
       <c r="AF42" s="9"/>
       <c r="AG42" s="9"/>
     </row>
     <row r="43" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W43" s="12"/>
+      <c r="W43" s="9"/>
       <c r="AC43" s="9"/>
       <c r="AF43" s="9"/>
       <c r="AG43" s="9"/>
     </row>
     <row r="44" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W44" s="12"/>
+      <c r="W44" s="9"/>
       <c r="AC44" s="9"/>
       <c r="AF44" s="9"/>
       <c r="AG44" s="9"/>
     </row>
     <row r="45" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W45" s="12"/>
+      <c r="W45" s="9"/>
       <c r="AC45" s="9"/>
       <c r="AF45" s="9"/>
       <c r="AG45" s="9"/>
     </row>
     <row r="46" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W46" s="12"/>
+      <c r="W46" s="9"/>
       <c r="AC46" s="9"/>
       <c r="AF46" s="9"/>
       <c r="AG46" s="9"/>
     </row>
     <row r="47" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W47" s="12"/>
+      <c r="W47" s="9"/>
       <c r="AC47" s="9"/>
       <c r="AF47" s="9"/>
       <c r="AG47" s="9"/>
     </row>
     <row r="48" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W48" s="12"/>
+      <c r="W48" s="9"/>
       <c r="AC48" s="9"/>
       <c r="AF48" s="9"/>
       <c r="AG48" s="9"/>
     </row>
     <row r="49" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W49" s="12"/>
+      <c r="W49" s="9"/>
       <c r="AC49" s="9"/>
       <c r="AF49" s="9"/>
       <c r="AG49" s="9"/>
     </row>
     <row r="50" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W50" s="12"/>
+      <c r="W50" s="9"/>
       <c r="AC50" s="9"/>
       <c r="AF50" s="9"/>
       <c r="AG50" s="9"/>
     </row>
     <row r="51" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W51" s="12"/>
+      <c r="W51" s="9"/>
       <c r="AC51" s="9"/>
       <c r="AF51" s="9"/>
       <c r="AG51" s="9"/>
     </row>
     <row r="52" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W52" s="12"/>
+      <c r="W52" s="9"/>
       <c r="AC52" s="9"/>
       <c r="AF52" s="9"/>
       <c r="AG52" s="9"/>
     </row>
     <row r="53" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W53" s="12"/>
+      <c r="W53" s="9"/>
       <c r="AC53" s="9"/>
       <c r="AF53" s="9"/>
       <c r="AG53" s="9"/>
     </row>
     <row r="54" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W54" s="12"/>
+      <c r="W54" s="9"/>
       <c r="AC54" s="9"/>
       <c r="AF54" s="9"/>
       <c r="AG54" s="9"/>
     </row>
     <row r="55" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W55" s="12"/>
+      <c r="W55" s="9"/>
       <c r="AC55" s="9"/>
       <c r="AF55" s="9"/>
       <c r="AG55" s="9"/>
     </row>
     <row r="56" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W56" s="12"/>
+      <c r="W56" s="9"/>
       <c r="AC56" s="9"/>
       <c r="AF56" s="9"/>
       <c r="AG56" s="9"/>
     </row>
     <row r="57" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W57" s="12"/>
+      <c r="W57" s="9"/>
       <c r="AC57" s="9"/>
       <c r="AF57" s="9"/>
       <c r="AG57" s="9"/>
     </row>
     <row r="58" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W58" s="12"/>
+      <c r="W58" s="9"/>
       <c r="AC58" s="9"/>
       <c r="AF58" s="9"/>
       <c r="AG58" s="9"/>
     </row>
     <row r="59" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W59" s="12"/>
+      <c r="W59" s="9"/>
       <c r="AC59" s="9"/>
       <c r="AF59" s="9"/>
       <c r="AG59" s="9"/>
     </row>
     <row r="60" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W60" s="12"/>
+      <c r="W60" s="9"/>
       <c r="AC60" s="9"/>
       <c r="AF60" s="9"/>
       <c r="AG60" s="9"/>
     </row>
     <row r="61" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W61" s="12"/>
+      <c r="W61" s="9"/>
       <c r="AC61" s="9"/>
       <c r="AF61" s="9"/>
       <c r="AG61" s="9"/>
     </row>
     <row r="62" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W62" s="12"/>
+      <c r="W62" s="9"/>
       <c r="AC62" s="9"/>
       <c r="AF62" s="9"/>
       <c r="AG62" s="9"/>
     </row>
     <row r="63" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W63" s="12"/>
+      <c r="W63" s="9"/>
       <c r="AC63" s="9"/>
       <c r="AF63" s="9"/>
       <c r="AG63" s="9"/>
     </row>
     <row r="64" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W64" s="12"/>
+      <c r="W64" s="9"/>
       <c r="AC64" s="9"/>
       <c r="AF64" s="9"/>
       <c r="AG64" s="9"/>
     </row>
     <row r="65" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W65" s="12"/>
+      <c r="W65" s="9"/>
       <c r="AC65" s="9"/>
       <c r="AF65" s="9"/>
       <c r="AG65" s="9"/>
     </row>
     <row r="66" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W66" s="12"/>
+      <c r="W66" s="9"/>
       <c r="AC66" s="9"/>
       <c r="AF66" s="9"/>
       <c r="AG66" s="9"/>
     </row>
     <row r="67" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W67" s="12"/>
+      <c r="W67" s="9"/>
       <c r="AC67" s="9"/>
       <c r="AF67" s="9"/>
       <c r="AG67" s="9"/>
     </row>
     <row r="68" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W68" s="12"/>
+      <c r="W68" s="9"/>
       <c r="AC68" s="9"/>
       <c r="AF68" s="9"/>
       <c r="AG68" s="9"/>
     </row>
     <row r="69" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W69" s="12"/>
+      <c r="W69" s="9"/>
       <c r="AC69" s="9"/>
       <c r="AF69" s="9"/>
       <c r="AG69" s="9"/>
     </row>
     <row r="70" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W70" s="12"/>
+      <c r="W70" s="9"/>
       <c r="AC70" s="9"/>
       <c r="AF70" s="9"/>
       <c r="AG70" s="9"/>
     </row>
     <row r="71" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W71" s="12"/>
+      <c r="W71" s="9"/>
       <c r="AC71" s="9"/>
       <c r="AF71" s="9"/>
       <c r="AG71" s="9"/>
     </row>
     <row r="72" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W72" s="12"/>
+      <c r="W72" s="9"/>
       <c r="AC72" s="9"/>
       <c r="AF72" s="9"/>
       <c r="AG72" s="9"/>
     </row>
     <row r="73" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W73" s="12"/>
+      <c r="W73" s="9"/>
       <c r="AC73" s="9"/>
       <c r="AF73" s="9"/>
       <c r="AG73" s="9"/>
     </row>
     <row r="74" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W74" s="12"/>
+      <c r="W74" s="9"/>
       <c r="AC74" s="9"/>
       <c r="AF74" s="9"/>
       <c r="AG74" s="9"/>
     </row>
     <row r="75" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W75" s="12"/>
+      <c r="W75" s="9"/>
       <c r="AC75" s="9"/>
       <c r="AF75" s="9"/>
       <c r="AG75" s="9"/>
     </row>
     <row r="76" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W76" s="12"/>
+      <c r="W76" s="9"/>
       <c r="AC76" s="9"/>
       <c r="AF76" s="9"/>
       <c r="AG76" s="9"/>
     </row>
     <row r="77" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W77" s="12"/>
+      <c r="W77" s="9"/>
       <c r="AC77" s="9"/>
       <c r="AF77" s="9"/>
       <c r="AG77" s="9"/>
     </row>
     <row r="78" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W78" s="12"/>
+      <c r="W78" s="9"/>
       <c r="AC78" s="9"/>
       <c r="AF78" s="9"/>
       <c r="AG78" s="9"/>
     </row>
     <row r="79" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W79" s="12"/>
+      <c r="W79" s="9"/>
       <c r="AC79" s="9"/>
       <c r="AF79" s="9"/>
       <c r="AG79" s="9"/>
     </row>
     <row r="80" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W80" s="12"/>
+      <c r="W80" s="9"/>
       <c r="AC80" s="9"/>
       <c r="AF80" s="9"/>
       <c r="AG80" s="9"/>
     </row>
     <row r="81" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W81" s="12"/>
+      <c r="W81" s="9"/>
       <c r="AC81" s="9"/>
       <c r="AF81" s="9"/>
       <c r="AG81" s="9"/>
     </row>
     <row r="82" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W82" s="12"/>
+      <c r="W82" s="9"/>
       <c r="AC82" s="9"/>
       <c r="AF82" s="9"/>
       <c r="AG82" s="9"/>
     </row>
     <row r="83" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W83" s="12"/>
+      <c r="W83" s="9"/>
       <c r="AC83" s="9"/>
       <c r="AF83" s="9"/>
       <c r="AG83" s="9"/>
     </row>
     <row r="84" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W84" s="12"/>
+      <c r="W84" s="9"/>
       <c r="AC84" s="9"/>
       <c r="AF84" s="9"/>
       <c r="AG84" s="9"/>
     </row>
     <row r="85" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W85" s="12"/>
+      <c r="W85" s="9"/>
       <c r="AC85" s="9"/>
       <c r="AF85" s="9"/>
       <c r="AG85" s="9"/>
     </row>
     <row r="86" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W86" s="12"/>
+      <c r="W86" s="9"/>
       <c r="AC86" s="9"/>
       <c r="AF86" s="9"/>
       <c r="AG86" s="9"/>
     </row>
     <row r="87" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W87" s="12"/>
+      <c r="W87" s="9"/>
       <c r="AC87" s="9"/>
       <c r="AF87" s="9"/>
       <c r="AG87" s="9"/>
     </row>
     <row r="88" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W88" s="12"/>
+      <c r="W88" s="9"/>
       <c r="AC88" s="9"/>
       <c r="AF88" s="9"/>
       <c r="AG88" s="9"/>
     </row>
     <row r="89" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W89" s="12"/>
+      <c r="W89" s="9"/>
       <c r="AC89" s="9"/>
       <c r="AF89" s="9"/>
       <c r="AG89" s="9"/>
     </row>
     <row r="90" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W90" s="12"/>
+      <c r="W90" s="9"/>
       <c r="AC90" s="9"/>
       <c r="AF90" s="9"/>
       <c r="AG90" s="9"/>
     </row>
     <row r="91" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W91" s="12"/>
+      <c r="W91" s="9"/>
       <c r="AC91" s="9"/>
       <c r="AF91" s="9"/>
       <c r="AG91" s="9"/>
     </row>
     <row r="92" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W92" s="12"/>
+      <c r="W92" s="9"/>
       <c r="AC92" s="9"/>
       <c r="AF92" s="9"/>
       <c r="AG92" s="9"/>
     </row>
     <row r="93" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W93" s="12"/>
+      <c r="W93" s="9"/>
       <c r="AC93" s="9"/>
       <c r="AF93" s="9"/>
       <c r="AG93" s="9"/>
     </row>
     <row r="94" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W94" s="12"/>
+      <c r="W94" s="9"/>
       <c r="AC94" s="9"/>
       <c r="AF94" s="9"/>
       <c r="AG94" s="9"/>
     </row>
     <row r="95" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W95" s="12"/>
+      <c r="W95" s="9"/>
       <c r="AC95" s="9"/>
       <c r="AF95" s="9"/>
       <c r="AG95" s="9"/>
     </row>
     <row r="96" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W96" s="12"/>
+      <c r="W96" s="9"/>
       <c r="AC96" s="9"/>
       <c r="AF96" s="9"/>
       <c r="AG96" s="9"/>
     </row>
     <row r="97" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W97" s="12"/>
+      <c r="W97" s="9"/>
       <c r="AC97" s="9"/>
       <c r="AF97" s="9"/>
       <c r="AG97" s="9"/>
     </row>
     <row r="98" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W98" s="12"/>
+      <c r="W98" s="9"/>
       <c r="AC98" s="9"/>
       <c r="AF98" s="9"/>
       <c r="AG98" s="9"/>
     </row>
     <row r="99" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W99" s="12"/>
+      <c r="W99" s="9"/>
       <c r="AC99" s="9"/>
       <c r="AF99" s="9"/>
       <c r="AG99" s="9"/>
     </row>
     <row r="100" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W100" s="12"/>
+      <c r="W100" s="9"/>
       <c r="AC100" s="9"/>
       <c r="AF100" s="9"/>
       <c r="AG100" s="9"/>
     </row>
     <row r="101" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W101" s="12"/>
+      <c r="W101" s="9"/>
       <c r="AC101" s="9"/>
       <c r="AF101" s="9"/>
       <c r="AG101" s="9"/>
     </row>
     <row r="102" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W102" s="12"/>
+      <c r="W102" s="9"/>
       <c r="AC102" s="9"/>
       <c r="AF102" s="9"/>
       <c r="AG102" s="9"/>
     </row>
     <row r="103" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W103" s="12"/>
+      <c r="W103" s="9"/>
       <c r="AC103" s="9"/>
       <c r="AF103" s="9"/>
       <c r="AG103" s="9"/>
     </row>
     <row r="104" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W104" s="12"/>
+      <c r="W104" s="9"/>
       <c r="AC104" s="9"/>
       <c r="AF104" s="9"/>
       <c r="AG104" s="9"/>
     </row>
     <row r="105" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W105" s="12"/>
+      <c r="W105" s="9"/>
       <c r="AC105" s="9"/>
       <c r="AF105" s="9"/>
       <c r="AG105" s="9"/>
     </row>
     <row r="106" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W106" s="12"/>
+      <c r="W106" s="9"/>
       <c r="AC106" s="9"/>
       <c r="AF106" s="9"/>
       <c r="AG106" s="9"/>
     </row>
     <row r="107" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W107" s="12"/>
+      <c r="W107" s="9"/>
       <c r="AC107" s="9"/>
       <c r="AF107" s="9"/>
       <c r="AG107" s="9"/>
     </row>
     <row r="108" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W108" s="12"/>
+      <c r="W108" s="9"/>
       <c r="AC108" s="9"/>
       <c r="AF108" s="9"/>
       <c r="AG108" s="9"/>
     </row>
     <row r="109" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W109" s="12"/>
+      <c r="W109" s="9"/>
       <c r="AC109" s="9"/>
       <c r="AF109" s="9"/>
       <c r="AG109" s="9"/>
     </row>
     <row r="110" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W110" s="12"/>
+      <c r="W110" s="9"/>
       <c r="AC110" s="9"/>
       <c r="AF110" s="9"/>
       <c r="AG110" s="9"/>
     </row>
     <row r="111" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W111" s="12"/>
+      <c r="W111" s="9"/>
       <c r="AC111" s="9"/>
       <c r="AF111" s="9"/>
       <c r="AG111" s="9"/>
     </row>
     <row r="112" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W112" s="12"/>
+      <c r="W112" s="9"/>
       <c r="AC112" s="9"/>
       <c r="AF112" s="9"/>
       <c r="AG112" s="9"/>
     </row>
     <row r="113" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W113" s="12"/>
+      <c r="W113" s="9"/>
       <c r="AC113" s="9"/>
       <c r="AF113" s="9"/>
       <c r="AG113" s="9"/>
     </row>
     <row r="114" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W114" s="12"/>
+      <c r="W114" s="9"/>
       <c r="AC114" s="9"/>
       <c r="AF114" s="9"/>
       <c r="AG114" s="9"/>
     </row>
     <row r="115" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W115" s="12"/>
+      <c r="W115" s="9"/>
       <c r="AC115" s="9"/>
       <c r="AF115" s="9"/>
       <c r="AG115" s="9"/>
     </row>
     <row r="116" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W116" s="12"/>
+      <c r="W116" s="9"/>
       <c r="AC116" s="9"/>
       <c r="AF116" s="9"/>
       <c r="AG116" s="9"/>
     </row>
     <row r="117" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W117" s="12"/>
+      <c r="W117" s="9"/>
       <c r="AC117" s="9"/>
       <c r="AF117" s="9"/>
       <c r="AG117" s="9"/>
     </row>
     <row r="118" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W118" s="12"/>
+      <c r="W118" s="9"/>
       <c r="AC118" s="9"/>
       <c r="AF118" s="9"/>
       <c r="AG118" s="9"/>
     </row>
     <row r="119" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W119" s="12"/>
+      <c r="W119" s="9"/>
       <c r="AC119" s="9"/>
       <c r="AF119" s="9"/>
       <c r="AG119" s="9"/>
     </row>
     <row r="120" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W120" s="12"/>
+      <c r="W120" s="9"/>
       <c r="AC120" s="9"/>
       <c r="AF120" s="9"/>
       <c r="AG120" s="9"/>
     </row>
     <row r="121" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W121" s="12"/>
+      <c r="W121" s="9"/>
       <c r="AC121" s="9"/>
       <c r="AF121" s="9"/>
       <c r="AG121" s="9"/>
     </row>
     <row r="122" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W122" s="12"/>
+      <c r="W122" s="9"/>
       <c r="AC122" s="9"/>
       <c r="AF122" s="9"/>
       <c r="AG122" s="9"/>
     </row>
     <row r="123" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W123" s="12"/>
+      <c r="W123" s="9"/>
       <c r="AC123" s="9"/>
       <c r="AF123" s="9"/>
       <c r="AG123" s="9"/>
     </row>
     <row r="124" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W124" s="12"/>
+      <c r="W124" s="9"/>
       <c r="AC124" s="9"/>
       <c r="AF124" s="9"/>
       <c r="AG124" s="9"/>
     </row>
     <row r="125" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W125" s="12"/>
+      <c r="W125" s="9"/>
       <c r="AC125" s="9"/>
       <c r="AF125" s="9"/>
       <c r="AG125" s="9"/>
     </row>
     <row r="126" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W126" s="12"/>
+      <c r="W126" s="9"/>
       <c r="AC126" s="9"/>
       <c r="AF126" s="9"/>
       <c r="AG126" s="9"/>
     </row>
     <row r="127" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W127" s="12"/>
+      <c r="W127" s="9"/>
       <c r="AC127" s="9"/>
       <c r="AF127" s="9"/>
       <c r="AG127" s="9"/>
     </row>
     <row r="128" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W128" s="12"/>
+      <c r="W128" s="9"/>
       <c r="AC128" s="9"/>
       <c r="AF128" s="9"/>
       <c r="AG128" s="9"/>
     </row>
     <row r="129" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W129" s="12"/>
+      <c r="W129" s="9"/>
       <c r="AC129" s="9"/>
       <c r="AF129" s="9"/>
       <c r="AG129" s="9"/>
     </row>
     <row r="130" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W130" s="12"/>
+      <c r="W130" s="9"/>
       <c r="AC130" s="9"/>
       <c r="AF130" s="9"/>
       <c r="AG130" s="9"/>
     </row>
     <row r="131" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W131" s="12"/>
+      <c r="W131" s="9"/>
       <c r="AC131" s="9"/>
       <c r="AF131" s="9"/>
       <c r="AG131" s="9"/>
     </row>
     <row r="132" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W132" s="12"/>
+      <c r="W132" s="9"/>
       <c r="AC132" s="9"/>
       <c r="AF132" s="9"/>
       <c r="AG132" s="9"/>
     </row>
     <row r="133" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W133" s="12"/>
+      <c r="W133" s="9"/>
       <c r="AC133" s="9"/>
       <c r="AF133" s="9"/>
       <c r="AG133" s="9"/>
     </row>
     <row r="134" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W134" s="12"/>
+      <c r="W134" s="9"/>
       <c r="AC134" s="9"/>
       <c r="AF134" s="9"/>
       <c r="AG134" s="9"/>
     </row>
     <row r="135" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W135" s="12"/>
+      <c r="W135" s="9"/>
       <c r="AC135" s="9"/>
       <c r="AF135" s="9"/>
       <c r="AG135" s="9"/>
     </row>
     <row r="136" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W136" s="12"/>
+      <c r="W136" s="9"/>
       <c r="AC136" s="9"/>
       <c r="AF136" s="9"/>
       <c r="AG136" s="9"/>
     </row>
     <row r="137" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W137" s="12"/>
+      <c r="W137" s="9"/>
       <c r="AC137" s="9"/>
       <c r="AF137" s="9"/>
       <c r="AG137" s="9"/>
     </row>
     <row r="138" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W138" s="12"/>
+      <c r="W138" s="9"/>
       <c r="AC138" s="9"/>
       <c r="AF138" s="9"/>
       <c r="AG138" s="9"/>
     </row>
     <row r="139" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W139" s="12"/>
+      <c r="W139" s="9"/>
       <c r="AC139" s="9"/>
       <c r="AF139" s="9"/>
       <c r="AG139" s="9"/>
     </row>
     <row r="140" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W140" s="12"/>
+      <c r="W140" s="9"/>
       <c r="AC140" s="9"/>
       <c r="AF140" s="9"/>
       <c r="AG140" s="9"/>
     </row>
     <row r="141" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W141" s="12"/>
+      <c r="W141" s="9"/>
       <c r="AC141" s="9"/>
       <c r="AF141" s="9"/>
       <c r="AG141" s="9"/>
     </row>
     <row r="142" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W142" s="12"/>
+      <c r="W142" s="9"/>
       <c r="AC142" s="9"/>
       <c r="AF142" s="9"/>
       <c r="AG142" s="9"/>
     </row>
     <row r="143" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W143" s="12"/>
+      <c r="W143" s="9"/>
       <c r="AC143" s="9"/>
       <c r="AF143" s="9"/>
       <c r="AG143" s="9"/>
     </row>
     <row r="144" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W144" s="12"/>
+      <c r="W144" s="9"/>
       <c r="AC144" s="9"/>
       <c r="AF144" s="9"/>
       <c r="AG144" s="9"/>
     </row>
     <row r="145" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W145" s="12"/>
+      <c r="W145" s="9"/>
       <c r="AC145" s="9"/>
       <c r="AF145" s="9"/>
       <c r="AG145" s="9"/>
     </row>
     <row r="146" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W146" s="12"/>
+      <c r="W146" s="9"/>
       <c r="AC146" s="9"/>
       <c r="AF146" s="9"/>
       <c r="AG146" s="9"/>
     </row>
     <row r="147" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W147" s="12"/>
+      <c r="W147" s="9"/>
       <c r="AC147" s="9"/>
       <c r="AF147" s="9"/>
       <c r="AG147" s="9"/>
     </row>
     <row r="148" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W148" s="12"/>
+      <c r="W148" s="9"/>
       <c r="AC148" s="9"/>
       <c r="AF148" s="9"/>
       <c r="AG148" s="9"/>
     </row>
     <row r="149" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W149" s="12"/>
+      <c r="W149" s="9"/>
       <c r="AC149" s="9"/>
       <c r="AF149" s="9"/>
       <c r="AG149" s="9"/>
     </row>
     <row r="150" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W150" s="12"/>
+      <c r="W150" s="9"/>
       <c r="AC150" s="9"/>
       <c r="AF150" s="9"/>
       <c r="AG150" s="9"/>
     </row>
     <row r="151" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W151" s="12"/>
+      <c r="W151" s="9"/>
       <c r="AC151" s="9"/>
       <c r="AF151" s="9"/>
       <c r="AG151" s="9"/>
     </row>
     <row r="152" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W152" s="12"/>
+      <c r="W152" s="9"/>
       <c r="AC152" s="9"/>
       <c r="AF152" s="9"/>
       <c r="AG152" s="9"/>
     </row>
     <row r="153" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W153" s="12"/>
+      <c r="W153" s="9"/>
       <c r="AC153" s="9"/>
       <c r="AF153" s="9"/>
       <c r="AG153" s="9"/>
     </row>
     <row r="154" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W154" s="12"/>
+      <c r="W154" s="9"/>
       <c r="AC154" s="9"/>
       <c r="AF154" s="9"/>
       <c r="AG154" s="9"/>
     </row>
     <row r="155" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W155" s="12"/>
+      <c r="W155" s="9"/>
       <c r="AC155" s="9"/>
       <c r="AF155" s="9"/>
       <c r="AG155" s="9"/>
     </row>
     <row r="156" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W156" s="12"/>
+      <c r="W156" s="9"/>
       <c r="AC156" s="9"/>
       <c r="AF156" s="9"/>
       <c r="AG156" s="9"/>
     </row>
     <row r="157" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W157" s="12"/>
+      <c r="W157" s="9"/>
       <c r="AC157" s="9"/>
       <c r="AF157" s="9"/>
       <c r="AG157" s="9"/>
     </row>
     <row r="158" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W158" s="12"/>
+      <c r="W158" s="9"/>
       <c r="AC158" s="9"/>
       <c r="AF158" s="9"/>
       <c r="AG158" s="9"/>
     </row>
     <row r="159" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W159" s="12"/>
+      <c r="W159" s="9"/>
       <c r="AC159" s="9"/>
       <c r="AF159" s="9"/>
       <c r="AG159" s="9"/>
     </row>
     <row r="160" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W160" s="12"/>
+      <c r="W160" s="9"/>
       <c r="AC160" s="9"/>
       <c r="AF160" s="9"/>
       <c r="AG160" s="9"/>
     </row>
     <row r="161" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W161" s="12"/>
+      <c r="W161" s="9"/>
       <c r="AC161" s="9"/>
       <c r="AF161" s="9"/>
       <c r="AG161" s="9"/>
     </row>
     <row r="162" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W162" s="12"/>
+      <c r="W162" s="9"/>
       <c r="AC162" s="9"/>
       <c r="AF162" s="9"/>
       <c r="AG162" s="9"/>
     </row>
     <row r="163" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W163" s="12"/>
+      <c r="W163" s="9"/>
       <c r="AC163" s="9"/>
       <c r="AF163" s="9"/>
       <c r="AG163" s="9"/>
     </row>
     <row r="164" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W164" s="12"/>
+      <c r="W164" s="9"/>
       <c r="AC164" s="9"/>
       <c r="AF164" s="9"/>
       <c r="AG164" s="9"/>
     </row>
     <row r="165" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W165" s="12"/>
+      <c r="W165" s="9"/>
       <c r="AC165" s="9"/>
       <c r="AF165" s="9"/>
       <c r="AG165" s="9"/>
     </row>
     <row r="166" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W166" s="12"/>
+      <c r="W166" s="9"/>
       <c r="AC166" s="9"/>
       <c r="AF166" s="9"/>
       <c r="AG166" s="9"/>
     </row>
     <row r="167" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W167" s="12"/>
+      <c r="W167" s="9"/>
       <c r="AC167" s="9"/>
       <c r="AF167" s="9"/>
       <c r="AG167" s="9"/>
     </row>
     <row r="168" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W168" s="12"/>
+      <c r="W168" s="9"/>
       <c r="AC168" s="9"/>
       <c r="AF168" s="9"/>
       <c r="AG168" s="9"/>
     </row>
     <row r="169" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W169" s="12"/>
+      <c r="W169" s="9"/>
       <c r="AC169" s="9"/>
       <c r="AF169" s="9"/>
       <c r="AG169" s="9"/>
     </row>
     <row r="170" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W170" s="12"/>
+      <c r="W170" s="9"/>
       <c r="AC170" s="9"/>
       <c r="AF170" s="9"/>
       <c r="AG170" s="9"/>
     </row>
     <row r="171" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W171" s="12"/>
+      <c r="W171" s="9"/>
       <c r="AC171" s="9"/>
       <c r="AF171" s="9"/>
       <c r="AG171" s="9"/>
     </row>
     <row r="172" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W172" s="12"/>
+      <c r="W172" s="9"/>
       <c r="AC172" s="9"/>
       <c r="AF172" s="9"/>
       <c r="AG172" s="9"/>
     </row>
     <row r="173" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W173" s="12"/>
+      <c r="W173" s="9"/>
       <c r="AC173" s="9"/>
       <c r="AF173" s="9"/>
       <c r="AG173" s="9"/>
     </row>
     <row r="174" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W174" s="12"/>
+      <c r="W174" s="9"/>
       <c r="AC174" s="9"/>
       <c r="AF174" s="9"/>
       <c r="AG174" s="9"/>
     </row>
     <row r="175" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W175" s="12"/>
+      <c r="W175" s="9"/>
       <c r="AC175" s="9"/>
       <c r="AF175" s="9"/>
       <c r="AG175" s="9"/>
     </row>
     <row r="176" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W176" s="12"/>
+      <c r="W176" s="9"/>
       <c r="AC176" s="9"/>
       <c r="AF176" s="9"/>
       <c r="AG176" s="9"/>
     </row>
     <row r="177" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W177" s="12"/>
+      <c r="W177" s="9"/>
       <c r="AC177" s="9"/>
       <c r="AF177" s="9"/>
       <c r="AG177" s="9"/>
     </row>
     <row r="178" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W178" s="12"/>
+      <c r="W178" s="9"/>
       <c r="AC178" s="9"/>
       <c r="AF178" s="9"/>
       <c r="AG178" s="9"/>
     </row>
     <row r="179" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W179" s="12"/>
+      <c r="W179" s="9"/>
       <c r="AC179" s="9"/>
       <c r="AF179" s="9"/>
       <c r="AG179" s="9"/>
     </row>
     <row r="180" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W180" s="12"/>
+      <c r="W180" s="9"/>
       <c r="AC180" s="9"/>
       <c r="AF180" s="9"/>
       <c r="AG180" s="9"/>
     </row>
     <row r="181" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W181" s="12"/>
+      <c r="W181" s="9"/>
       <c r="AC181" s="9"/>
       <c r="AF181" s="9"/>
       <c r="AG181" s="9"/>
     </row>
     <row r="182" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W182" s="12"/>
+      <c r="W182" s="9"/>
       <c r="AC182" s="9"/>
       <c r="AF182" s="9"/>
       <c r="AG182" s="9"/>
     </row>
     <row r="183" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W183" s="12"/>
+      <c r="W183" s="9"/>
       <c r="AC183" s="9"/>
       <c r="AF183" s="9"/>
       <c r="AG183" s="9"/>
     </row>
     <row r="184" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W184" s="12"/>
+      <c r="W184" s="9"/>
       <c r="AC184" s="9"/>
       <c r="AF184" s="9"/>
       <c r="AG184" s="9"/>
     </row>
     <row r="185" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W185" s="12"/>
+      <c r="W185" s="9"/>
       <c r="AC185" s="9"/>
       <c r="AF185" s="9"/>
       <c r="AG185" s="9"/>
     </row>
     <row r="186" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W186" s="12"/>
+      <c r="W186" s="9"/>
       <c r="AC186" s="9"/>
       <c r="AF186" s="9"/>
       <c r="AG186" s="9"/>
     </row>
     <row r="187" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W187" s="12"/>
+      <c r="W187" s="9"/>
       <c r="AC187" s="9"/>
       <c r="AF187" s="9"/>
       <c r="AG187" s="9"/>
     </row>
     <row r="188" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W188" s="12"/>
+      <c r="W188" s="9"/>
       <c r="AC188" s="9"/>
       <c r="AF188" s="9"/>
       <c r="AG188" s="9"/>
     </row>
     <row r="189" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W189" s="12"/>
+      <c r="W189" s="9"/>
       <c r="AC189" s="9"/>
       <c r="AF189" s="9"/>
       <c r="AG189" s="9"/>
     </row>
     <row r="190" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W190" s="12"/>
+      <c r="W190" s="9"/>
       <c r="AC190" s="9"/>
       <c r="AF190" s="9"/>
       <c r="AG190" s="9"/>
     </row>
     <row r="191" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W191" s="12"/>
+      <c r="W191" s="9"/>
       <c r="AC191" s="9"/>
       <c r="AF191" s="9"/>
       <c r="AG191" s="9"/>
     </row>
     <row r="192" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W192" s="12"/>
+      <c r="W192" s="9"/>
       <c r="AC192" s="9"/>
       <c r="AF192" s="9"/>
       <c r="AG192" s="9"/>
     </row>
     <row r="193" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W193" s="12"/>
+      <c r="W193" s="9"/>
       <c r="AC193" s="9"/>
       <c r="AF193" s="9"/>
       <c r="AG193" s="9"/>
     </row>
     <row r="194" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W194" s="12"/>
+      <c r="W194" s="9"/>
       <c r="AC194" s="9"/>
       <c r="AF194" s="9"/>
       <c r="AG194" s="9"/>
     </row>
     <row r="195" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W195" s="12"/>
+      <c r="W195" s="9"/>
       <c r="AC195" s="9"/>
       <c r="AF195" s="9"/>
       <c r="AG195" s="9"/>
     </row>
     <row r="196" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W196" s="12"/>
+      <c r="W196" s="9"/>
       <c r="AC196" s="9"/>
       <c r="AF196" s="9"/>
       <c r="AG196" s="9"/>
     </row>
     <row r="197" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W197" s="12"/>
+      <c r="W197" s="9"/>
       <c r="AC197" s="9"/>
       <c r="AF197" s="9"/>
       <c r="AG197" s="9"/>
     </row>
     <row r="198" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W198" s="12"/>
+      <c r="W198" s="9"/>
       <c r="AC198" s="9"/>
       <c r="AF198" s="9"/>
       <c r="AG198" s="9"/>
     </row>
     <row r="199" spans="23:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W199" s="12"/>
+      <c r="W199" s="9"/>
       <c r="AC199" s="9"/>
       <c r="AF199" s="9"/>
       <c r="AG199" s="9"/>

</xml_diff>

<commit_message>
revision on the study outcome
</commit_message>
<xml_diff>
--- a/Data Extraction Sheet.xlsx
+++ b/Data Extraction Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/rw3031_cumc_columbia_edu/Documents/Documents/EveryBreathMatters/systematic review/lungcancer_tech_slr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="395" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759ADE5E-B86B-459B-A44F-381F7197B621}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D3BBD9D-E78B-481C-8788-A5ABEEB45AA9}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sheet" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="635">
   <si>
     <t>Title</t>
   </si>
@@ -2139,9 +2139,6 @@
   </si>
   <si>
     <t>monitoring and tracking,communication and coordination,education and information delivery</t>
-  </si>
-  <si>
-    <t>Pre-treatment,Post-treatment</t>
   </si>
 </sst>
 </file>
@@ -2690,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView tabSelected="1" topLeftCell="AB12" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3655,7 +3652,7 @@
         <v>540</v>
       </c>
       <c r="AF9" s="9" t="s">
-        <v>635</v>
+        <v>561</v>
       </c>
       <c r="AG9" s="9" t="s">
         <v>570</v>

</xml_diff>

<commit_message>
update on technology challenge
</commit_message>
<xml_diff>
--- a/Data Extraction Sheet.xlsx
+++ b/Data Extraction Sheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/rw3031_cumc_columbia_edu/Documents/Documents/EveryBreathMatters/systematic review/lungcancer_tech_slr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D3BBD9D-E78B-481C-8788-A5ABEEB45AA9}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{B590317F-974E-4B35-BB01-69E387BE72C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{611B35E8-772E-4C16-8F3F-71EDCC0EE723}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sheet" sheetId="1" r:id="rId1"/>
     <sheet name="variable name" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="637">
   <si>
     <t>Title</t>
   </si>
@@ -2139,6 +2140,12 @@
   </si>
   <si>
     <t>monitoring and tracking,communication and coordination,education and information delivery</t>
+  </si>
+  <si>
+    <t>To investigate the feasibility, acceptability, safety, and potential efficacy of inspiratory muscle training (IMT) and walking promotion to disrupt a postulated “dyspnea-inactivity” spiral.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage </t>
   </si>
 </sst>
 </file>
@@ -2687,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB12" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AF30" sqref="AF30"/>
+    <sheetView topLeftCell="AB1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection sqref="A1:AH30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56367,4 +56374,2027 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DF66AC-F12A-40A3-9D25-6DBBEDD703E7}">
+  <dimension ref="A1:AB24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="4" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="23.90625" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" customWidth="1"/>
+    <col min="13" max="13" width="38" customWidth="1"/>
+    <col min="14" max="14" width="19.36328125" customWidth="1"/>
+    <col min="18" max="18" width="21.54296875" customWidth="1"/>
+    <col min="19" max="19" width="36.08984375" customWidth="1"/>
+    <col min="20" max="20" width="24.1796875" customWidth="1"/>
+    <col min="21" max="21" width="18.7265625" customWidth="1"/>
+    <col min="28" max="28" width="20.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>2023</v>
+      </c>
+      <c r="D2" t="s">
+        <v>635</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>518</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>406</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s">
+        <v>539</v>
+      </c>
+      <c r="S2" t="s">
+        <v>564</v>
+      </c>
+      <c r="T2" t="s">
+        <v>504</v>
+      </c>
+      <c r="U2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
+        <v>561</v>
+      </c>
+      <c r="W2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>2024</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>510</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s">
+        <v>442</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" t="s">
+        <v>565</v>
+      </c>
+      <c r="T3" t="s">
+        <v>559</v>
+      </c>
+      <c r="U3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" t="s">
+        <v>560</v>
+      </c>
+      <c r="W3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" t="s">
+        <v>552</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <v>2019</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" t="s">
+        <v>384</v>
+      </c>
+      <c r="O4" t="s">
+        <v>406</v>
+      </c>
+      <c r="P4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" t="s">
+        <v>566</v>
+      </c>
+      <c r="T4" t="s">
+        <v>559</v>
+      </c>
+      <c r="U4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" t="s">
+        <v>560</v>
+      </c>
+      <c r="W4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5">
+        <v>2014</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N5" t="s">
+        <v>126</v>
+      </c>
+      <c r="O5" t="s">
+        <v>406</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" t="s">
+        <v>541</v>
+      </c>
+      <c r="S5" t="s">
+        <v>568</v>
+      </c>
+      <c r="T5" t="s">
+        <v>505</v>
+      </c>
+      <c r="U5" t="s">
+        <v>549</v>
+      </c>
+      <c r="V5" t="s">
+        <v>562</v>
+      </c>
+      <c r="W5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" t="s">
+        <v>630</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" t="s">
+        <v>512</v>
+      </c>
+      <c r="H6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" t="s">
+        <v>520</v>
+      </c>
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N6" t="s">
+        <v>136</v>
+      </c>
+      <c r="O6" t="s">
+        <v>406</v>
+      </c>
+      <c r="P6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" t="s">
+        <v>542</v>
+      </c>
+      <c r="S6" t="s">
+        <v>569</v>
+      </c>
+      <c r="T6" t="s">
+        <v>505</v>
+      </c>
+      <c r="U6" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" t="s">
+        <v>560</v>
+      </c>
+      <c r="W6" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" t="s">
+        <v>556</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7">
+        <v>2021</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" t="s">
+        <v>509</v>
+      </c>
+      <c r="I7" t="s">
+        <v>519</v>
+      </c>
+      <c r="J7" t="s">
+        <v>144</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" t="s">
+        <v>145</v>
+      </c>
+      <c r="N7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" t="s">
+        <v>406</v>
+      </c>
+      <c r="P7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" t="s">
+        <v>543</v>
+      </c>
+      <c r="S7" t="s">
+        <v>565</v>
+      </c>
+      <c r="T7" t="s">
+        <v>506</v>
+      </c>
+      <c r="U7" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" t="s">
+        <v>560</v>
+      </c>
+      <c r="W7" t="s">
+        <v>40</v>
+      </c>
+      <c r="X7" t="s">
+        <v>557</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M8" t="s">
+        <v>170</v>
+      </c>
+      <c r="N8" t="s">
+        <v>173</v>
+      </c>
+      <c r="O8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" t="s">
+        <v>174</v>
+      </c>
+      <c r="R8" t="s">
+        <v>540</v>
+      </c>
+      <c r="S8" t="s">
+        <v>570</v>
+      </c>
+      <c r="T8" t="s">
+        <v>504</v>
+      </c>
+      <c r="U8" t="s">
+        <v>549</v>
+      </c>
+      <c r="V8" t="s">
+        <v>561</v>
+      </c>
+      <c r="W8" t="s">
+        <v>177</v>
+      </c>
+      <c r="X8" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9">
+        <v>2017</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" t="s">
+        <v>154</v>
+      </c>
+      <c r="J9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M9" t="s">
+        <v>156</v>
+      </c>
+      <c r="N9" t="s">
+        <v>155</v>
+      </c>
+      <c r="O9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" t="s">
+        <v>539</v>
+      </c>
+      <c r="S9" t="s">
+        <v>571</v>
+      </c>
+      <c r="T9" t="s">
+        <v>504</v>
+      </c>
+      <c r="U9" t="s">
+        <v>549</v>
+      </c>
+      <c r="V9" t="s">
+        <v>560</v>
+      </c>
+      <c r="W9" t="s">
+        <v>40</v>
+      </c>
+      <c r="X9" t="s">
+        <v>553</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10">
+        <v>2007</v>
+      </c>
+      <c r="D10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" t="s">
+        <v>454</v>
+      </c>
+      <c r="I10" t="s">
+        <v>522</v>
+      </c>
+      <c r="J10" t="s">
+        <v>521</v>
+      </c>
+      <c r="K10" t="s">
+        <v>190</v>
+      </c>
+      <c r="L10" t="s">
+        <v>169</v>
+      </c>
+      <c r="M10" t="s">
+        <v>193</v>
+      </c>
+      <c r="N10" t="s">
+        <v>186</v>
+      </c>
+      <c r="O10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" t="s">
+        <v>55</v>
+      </c>
+      <c r="S10" t="s">
+        <v>572</v>
+      </c>
+      <c r="T10" t="s">
+        <v>507</v>
+      </c>
+      <c r="U10" t="s">
+        <v>549</v>
+      </c>
+      <c r="V10" t="s">
+        <v>560</v>
+      </c>
+      <c r="W10" t="s">
+        <v>188</v>
+      </c>
+      <c r="X10" t="s">
+        <v>554</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11">
+        <v>2024</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" t="s">
+        <v>218</v>
+      </c>
+      <c r="J11" t="s">
+        <v>219</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N11" t="s">
+        <v>225</v>
+      </c>
+      <c r="O11" t="s">
+        <v>442</v>
+      </c>
+      <c r="P11" t="s">
+        <v>226</v>
+      </c>
+      <c r="R11" t="s">
+        <v>55</v>
+      </c>
+      <c r="S11" t="s">
+        <v>572</v>
+      </c>
+      <c r="T11" t="s">
+        <v>504</v>
+      </c>
+      <c r="U11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" t="s">
+        <v>560</v>
+      </c>
+      <c r="W11" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" t="s">
+        <v>557</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12">
+        <v>2018</v>
+      </c>
+      <c r="D12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" t="s">
+        <v>454</v>
+      </c>
+      <c r="I12" t="s">
+        <v>522</v>
+      </c>
+      <c r="J12" t="s">
+        <v>235</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" t="s">
+        <v>237</v>
+      </c>
+      <c r="M12" t="s">
+        <v>239</v>
+      </c>
+      <c r="N12" t="s">
+        <v>236</v>
+      </c>
+      <c r="O12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" t="s">
+        <v>544</v>
+      </c>
+      <c r="S12" t="s">
+        <v>574</v>
+      </c>
+      <c r="T12" t="s">
+        <v>506</v>
+      </c>
+      <c r="U12" t="s">
+        <v>39</v>
+      </c>
+      <c r="V12" t="s">
+        <v>560</v>
+      </c>
+      <c r="W12" t="s">
+        <v>241</v>
+      </c>
+      <c r="X12" t="s">
+        <v>555</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13">
+        <v>2017</v>
+      </c>
+      <c r="D13" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F13" t="s">
+        <v>254</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" t="s">
+        <v>523</v>
+      </c>
+      <c r="J13" t="s">
+        <v>255</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" t="s">
+        <v>109</v>
+      </c>
+      <c r="M13" t="s">
+        <v>249</v>
+      </c>
+      <c r="N13" t="s">
+        <v>250</v>
+      </c>
+      <c r="O13" t="s">
+        <v>406</v>
+      </c>
+      <c r="P13" t="s">
+        <v>40</v>
+      </c>
+      <c r="R13" t="s">
+        <v>539</v>
+      </c>
+      <c r="S13" t="s">
+        <v>565</v>
+      </c>
+      <c r="T13" t="s">
+        <v>559</v>
+      </c>
+      <c r="U13" t="s">
+        <v>39</v>
+      </c>
+      <c r="V13" t="s">
+        <v>561</v>
+      </c>
+      <c r="W13" t="s">
+        <v>40</v>
+      </c>
+      <c r="X13" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>259</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>258</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>2024</v>
+      </c>
+      <c r="D14" t="s">
+        <v>261</v>
+      </c>
+      <c r="E14" t="s">
+        <v>270</v>
+      </c>
+      <c r="F14" t="s">
+        <v>262</v>
+      </c>
+      <c r="G14" t="s">
+        <v>513</v>
+      </c>
+      <c r="H14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" t="s">
+        <v>524</v>
+      </c>
+      <c r="J14" t="s">
+        <v>271</v>
+      </c>
+      <c r="K14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" t="s">
+        <v>263</v>
+      </c>
+      <c r="M14" t="s">
+        <v>264</v>
+      </c>
+      <c r="N14" t="s">
+        <v>265</v>
+      </c>
+      <c r="O14" t="s">
+        <v>442</v>
+      </c>
+      <c r="P14" t="s">
+        <v>40</v>
+      </c>
+      <c r="R14" t="s">
+        <v>55</v>
+      </c>
+      <c r="S14" t="s">
+        <v>575</v>
+      </c>
+      <c r="T14" t="s">
+        <v>559</v>
+      </c>
+      <c r="U14" t="s">
+        <v>549</v>
+      </c>
+      <c r="V14" t="s">
+        <v>560</v>
+      </c>
+      <c r="W14" t="s">
+        <v>40</v>
+      </c>
+      <c r="X14" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15">
+        <v>2014</v>
+      </c>
+      <c r="D15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E15" t="s">
+        <v>277</v>
+      </c>
+      <c r="F15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G15" t="s">
+        <v>514</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" t="s">
+        <v>522</v>
+      </c>
+      <c r="J15" t="s">
+        <v>279</v>
+      </c>
+      <c r="K15" t="s">
+        <v>283</v>
+      </c>
+      <c r="L15" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" t="s">
+        <v>285</v>
+      </c>
+      <c r="N15" t="s">
+        <v>284</v>
+      </c>
+      <c r="O15" t="s">
+        <v>538</v>
+      </c>
+      <c r="P15" t="s">
+        <v>40</v>
+      </c>
+      <c r="R15" t="s">
+        <v>544</v>
+      </c>
+      <c r="S15" t="s">
+        <v>568</v>
+      </c>
+      <c r="T15" t="s">
+        <v>505</v>
+      </c>
+      <c r="U15" t="s">
+        <v>39</v>
+      </c>
+      <c r="V15" t="s">
+        <v>562</v>
+      </c>
+      <c r="W15" t="s">
+        <v>40</v>
+      </c>
+      <c r="X15" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>288</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>291</v>
+      </c>
+      <c r="C16">
+        <v>2016</v>
+      </c>
+      <c r="D16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E16" t="s">
+        <v>293</v>
+      </c>
+      <c r="F16" t="s">
+        <v>294</v>
+      </c>
+      <c r="G16" t="s">
+        <v>515</v>
+      </c>
+      <c r="H16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" t="s">
+        <v>525</v>
+      </c>
+      <c r="J16" t="s">
+        <v>295</v>
+      </c>
+      <c r="K16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" t="s">
+        <v>296</v>
+      </c>
+      <c r="M16" t="s">
+        <v>303</v>
+      </c>
+      <c r="N16" t="s">
+        <v>301</v>
+      </c>
+      <c r="O16" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" t="s">
+        <v>40</v>
+      </c>
+      <c r="R16" t="s">
+        <v>540</v>
+      </c>
+      <c r="S16" t="s">
+        <v>572</v>
+      </c>
+      <c r="T16" t="s">
+        <v>505</v>
+      </c>
+      <c r="U16" t="s">
+        <v>39</v>
+      </c>
+      <c r="V16" t="s">
+        <v>561</v>
+      </c>
+      <c r="W16" t="s">
+        <v>40</v>
+      </c>
+      <c r="X16" t="s">
+        <v>556</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>299</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>304</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17">
+        <v>2024</v>
+      </c>
+      <c r="D17" t="s">
+        <v>337</v>
+      </c>
+      <c r="E17" t="s">
+        <v>338</v>
+      </c>
+      <c r="F17" t="s">
+        <v>339</v>
+      </c>
+      <c r="G17" t="s">
+        <v>516</v>
+      </c>
+      <c r="H17" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" t="s">
+        <v>526</v>
+      </c>
+      <c r="J17" t="s">
+        <v>340</v>
+      </c>
+      <c r="K17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
+        <v>169</v>
+      </c>
+      <c r="M17" t="s">
+        <v>346</v>
+      </c>
+      <c r="N17" t="s">
+        <v>341</v>
+      </c>
+      <c r="O17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" t="s">
+        <v>40</v>
+      </c>
+      <c r="R17" t="s">
+        <v>544</v>
+      </c>
+      <c r="S17" t="s">
+        <v>572</v>
+      </c>
+      <c r="T17" t="s">
+        <v>504</v>
+      </c>
+      <c r="U17" t="s">
+        <v>39</v>
+      </c>
+      <c r="V17" t="s">
+        <v>560</v>
+      </c>
+      <c r="W17" t="s">
+        <v>182</v>
+      </c>
+      <c r="X17" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>348</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>347</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18">
+        <v>2017</v>
+      </c>
+      <c r="D18" t="s">
+        <v>349</v>
+      </c>
+      <c r="E18" t="s">
+        <v>350</v>
+      </c>
+      <c r="F18" t="s">
+        <v>353</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" t="s">
+        <v>527</v>
+      </c>
+      <c r="J18" t="s">
+        <v>354</v>
+      </c>
+      <c r="K18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" t="s">
+        <v>355</v>
+      </c>
+      <c r="N18" t="s">
+        <v>351</v>
+      </c>
+      <c r="O18" t="s">
+        <v>406</v>
+      </c>
+      <c r="P18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R18" t="s">
+        <v>545</v>
+      </c>
+      <c r="S18" t="s">
+        <v>576</v>
+      </c>
+      <c r="T18" t="s">
+        <v>559</v>
+      </c>
+      <c r="U18" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" t="s">
+        <v>561</v>
+      </c>
+      <c r="W18" t="s">
+        <v>40</v>
+      </c>
+      <c r="X18" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>359</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>352</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19">
+        <v>2017</v>
+      </c>
+      <c r="D19" t="s">
+        <v>362</v>
+      </c>
+      <c r="E19" t="s">
+        <v>364</v>
+      </c>
+      <c r="F19" t="s">
+        <v>365</v>
+      </c>
+      <c r="G19" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" t="s">
+        <v>366</v>
+      </c>
+      <c r="I19" t="s">
+        <v>154</v>
+      </c>
+      <c r="J19" t="s">
+        <v>367</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" t="s">
+        <v>169</v>
+      </c>
+      <c r="M19" t="s">
+        <v>368</v>
+      </c>
+      <c r="N19" t="s">
+        <v>369</v>
+      </c>
+      <c r="O19" t="s">
+        <v>406</v>
+      </c>
+      <c r="P19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19" t="s">
+        <v>55</v>
+      </c>
+      <c r="S19" t="s">
+        <v>576</v>
+      </c>
+      <c r="T19" t="s">
+        <v>559</v>
+      </c>
+      <c r="U19" t="s">
+        <v>39</v>
+      </c>
+      <c r="V19" t="s">
+        <v>560</v>
+      </c>
+      <c r="W19" t="s">
+        <v>40</v>
+      </c>
+      <c r="X19" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>363</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>372</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>373</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20">
+        <v>2017</v>
+      </c>
+      <c r="D20" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20" t="s">
+        <v>386</v>
+      </c>
+      <c r="F20" t="s">
+        <v>387</v>
+      </c>
+      <c r="G20" t="s">
+        <v>205</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" t="s">
+        <v>519</v>
+      </c>
+      <c r="J20" t="s">
+        <v>388</v>
+      </c>
+      <c r="K20" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" t="s">
+        <v>88</v>
+      </c>
+      <c r="M20" t="s">
+        <v>393</v>
+      </c>
+      <c r="N20" t="s">
+        <v>389</v>
+      </c>
+      <c r="O20" t="s">
+        <v>406</v>
+      </c>
+      <c r="P20" t="s">
+        <v>40</v>
+      </c>
+      <c r="R20" t="s">
+        <v>539</v>
+      </c>
+      <c r="S20" t="s">
+        <v>564</v>
+      </c>
+      <c r="T20" t="s">
+        <v>505</v>
+      </c>
+      <c r="U20" t="s">
+        <v>39</v>
+      </c>
+      <c r="V20" t="s">
+        <v>560</v>
+      </c>
+      <c r="W20" t="s">
+        <v>40</v>
+      </c>
+      <c r="X20" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>391</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>397</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>398</v>
+      </c>
+      <c r="C21">
+        <v>2021</v>
+      </c>
+      <c r="D21" t="s">
+        <v>399</v>
+      </c>
+      <c r="E21" t="s">
+        <v>400</v>
+      </c>
+      <c r="F21" t="s">
+        <v>403</v>
+      </c>
+      <c r="G21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" t="s">
+        <v>525</v>
+      </c>
+      <c r="J21" t="s">
+        <v>401</v>
+      </c>
+      <c r="K21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" t="s">
+        <v>169</v>
+      </c>
+      <c r="M21" t="s">
+        <v>404</v>
+      </c>
+      <c r="N21" t="s">
+        <v>405</v>
+      </c>
+      <c r="O21" t="s">
+        <v>406</v>
+      </c>
+      <c r="P21" t="s">
+        <v>40</v>
+      </c>
+      <c r="R21" t="s">
+        <v>546</v>
+      </c>
+      <c r="S21" t="s">
+        <v>571</v>
+      </c>
+      <c r="T21" t="s">
+        <v>504</v>
+      </c>
+      <c r="U21" t="s">
+        <v>549</v>
+      </c>
+      <c r="V21" t="s">
+        <v>562</v>
+      </c>
+      <c r="W21" t="s">
+        <v>182</v>
+      </c>
+      <c r="X21" t="s">
+        <v>557</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>409</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>411</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22">
+        <v>2007</v>
+      </c>
+      <c r="D22" t="s">
+        <v>419</v>
+      </c>
+      <c r="E22" t="s">
+        <v>420</v>
+      </c>
+      <c r="F22" t="s">
+        <v>421</v>
+      </c>
+      <c r="G22" t="s">
+        <v>189</v>
+      </c>
+      <c r="H22" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" t="s">
+        <v>154</v>
+      </c>
+      <c r="J22" t="s">
+        <v>422</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" t="s">
+        <v>169</v>
+      </c>
+      <c r="M22" t="s">
+        <v>424</v>
+      </c>
+      <c r="N22" t="s">
+        <v>425</v>
+      </c>
+      <c r="O22" t="s">
+        <v>406</v>
+      </c>
+      <c r="P22" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" t="s">
+        <v>55</v>
+      </c>
+      <c r="S22" t="s">
+        <v>573</v>
+      </c>
+      <c r="T22" t="s">
+        <v>504</v>
+      </c>
+      <c r="U22" t="s">
+        <v>39</v>
+      </c>
+      <c r="V22" t="s">
+        <v>560</v>
+      </c>
+      <c r="W22" t="s">
+        <v>182</v>
+      </c>
+      <c r="X22" t="s">
+        <v>557</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>428</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>430</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>433</v>
+      </c>
+      <c r="C23">
+        <v>2023</v>
+      </c>
+      <c r="D23" t="s">
+        <v>434</v>
+      </c>
+      <c r="E23" t="s">
+        <v>435</v>
+      </c>
+      <c r="F23" t="s">
+        <v>436</v>
+      </c>
+      <c r="G23" t="s">
+        <v>189</v>
+      </c>
+      <c r="H23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" t="s">
+        <v>531</v>
+      </c>
+      <c r="J23" t="s">
+        <v>438</v>
+      </c>
+      <c r="K23" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" t="s">
+        <v>169</v>
+      </c>
+      <c r="M23" t="s">
+        <v>440</v>
+      </c>
+      <c r="N23" t="s">
+        <v>441</v>
+      </c>
+      <c r="O23" t="s">
+        <v>442</v>
+      </c>
+      <c r="P23" t="s">
+        <v>40</v>
+      </c>
+      <c r="R23" t="s">
+        <v>580</v>
+      </c>
+      <c r="S23" t="s">
+        <v>577</v>
+      </c>
+      <c r="T23" t="s">
+        <v>559</v>
+      </c>
+      <c r="U23" t="s">
+        <v>39</v>
+      </c>
+      <c r="V23" t="s">
+        <v>560</v>
+      </c>
+      <c r="W23" t="s">
+        <v>182</v>
+      </c>
+      <c r="X23" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>465</v>
+      </c>
+      <c r="C24">
+        <v>2021</v>
+      </c>
+      <c r="D24" t="s">
+        <v>466</v>
+      </c>
+      <c r="E24" t="s">
+        <v>467</v>
+      </c>
+      <c r="F24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G24" t="s">
+        <v>517</v>
+      </c>
+      <c r="H24" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" t="s">
+        <v>154</v>
+      </c>
+      <c r="J24" t="s">
+        <v>470</v>
+      </c>
+      <c r="K24" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M24" t="s">
+        <v>472</v>
+      </c>
+      <c r="N24" t="s">
+        <v>471</v>
+      </c>
+      <c r="O24" t="s">
+        <v>442</v>
+      </c>
+      <c r="P24" t="s">
+        <v>40</v>
+      </c>
+      <c r="R24" t="s">
+        <v>547</v>
+      </c>
+      <c r="S24" t="s">
+        <v>578</v>
+      </c>
+      <c r="T24" t="s">
+        <v>504</v>
+      </c>
+      <c r="U24" t="s">
+        <v>549</v>
+      </c>
+      <c r="V24" t="s">
+        <v>560</v>
+      </c>
+      <c r="W24" t="s">
+        <v>182</v>
+      </c>
+      <c r="X24" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>476</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>478</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>475</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>477</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>